<commit_message>
working on all_averages with HP
</commit_message>
<xml_diff>
--- a/data/general/all_averages.xlsx
+++ b/data/general/all_averages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="18740" windowHeight="17540"/>
+    <workbookView xWindow="3480" yWindow="0" windowWidth="25080" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="26">
   <si>
     <t>Company</t>
   </si>
@@ -141,18 +141,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -164,9 +158,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="212">
+  <cellStyleXfs count="218">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -384,12 +384,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="212">
+  <cellStyles count="218">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -495,6 +495,9 @@
     <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="211" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -600,6 +603,9 @@
     <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="208" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="210" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="212" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="214" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="216" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1182,7 +1188,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1190,10 +1196,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N102"/>
+  <dimension ref="A1:M107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="E102" sqref="E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1207,8 +1213,8 @@
     <col min="7" max="7" width="15.6640625" customWidth="1"/>
     <col min="8" max="9" width="14.6640625" customWidth="1"/>
     <col min="10" max="10" width="8.5" customWidth="1"/>
-    <col min="11" max="11" width="20.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.5" style="6" customWidth="1"/>
+    <col min="11" max="11" width="20.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.5" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -1242,10 +1248,10 @@
       <c r="J1" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>25</v>
       </c>
       <c r="M1" t="s">
@@ -1289,14 +1295,14 @@
         <f>[1]apple_averages!I12</f>
         <v>0.75669047547119428</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="5">
         <f>[1]apple_averages!J12</f>
         <v>-1.5800000000000002E-2</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K2" s="5">
         <v>-2.977761025254444E-2</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="5">
         <v>-4.7719562759140688E-2</v>
       </c>
       <c r="M2" t="s">
@@ -1340,14 +1346,14 @@
         <f>[1]apple_averages!I24</f>
         <v>0.7795316656508281</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <f>[1]apple_averages!J24</f>
         <v>-4.2299999999999997E-2</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="5">
         <v>-5.6367112810707498E-2</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="5">
         <v>-0.12321223709369022</v>
       </c>
       <c r="M3" t="s">
@@ -1391,14 +1397,14 @@
         <f>[1]apple_averages!I38</f>
         <v>0.72656414989418927</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="5">
         <f>[1]apple_averages!J38</f>
         <v>4.1200000000000001E-2</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <v>7.001309471846362E-2</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="5">
         <v>1.9380183326058509E-2</v>
       </c>
       <c r="M4" t="s">
@@ -1442,11 +1448,11 @@
         <f>[1]apple_averages!I51</f>
         <v>0.3759358527084678</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <f>[1]apple_averages!J51</f>
         <v>-6.5699999999999995E-2</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="5">
         <v>-5.5105510551055059E-2</v>
       </c>
       <c r="L5" s="4">
@@ -1493,11 +1499,11 @@
         <f>[1]apple_averages!I64</f>
         <v>-0.75202448372129327</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <f>[1]apple_averages!J64</f>
         <v>-6.2600000000000003E-2</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="5">
         <v>-8.7877335888835506E-2</v>
       </c>
       <c r="L6" s="4">
@@ -1544,11 +1550,11 @@
         <f>[1]apple_averages!I77</f>
         <v>0.33644991917489508</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="5">
         <f>[1]apple_averages!J77</f>
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="5">
         <v>8.079031757525601E-2</v>
       </c>
       <c r="L7" s="4">
@@ -1595,11 +1601,11 @@
         <f>[1]apple_averages!I90</f>
         <v>0.58187631820128038</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="5">
         <f>[1]apple_averages!J90</f>
         <v>-2.2499999999999999E-2</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="5">
         <v>-5.7167019027484223E-2</v>
       </c>
       <c r="L8" s="4">
@@ -1646,11 +1652,11 @@
         <f>[1]apple_averages!I104</f>
         <v>-0.27665766882768922</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="5">
         <f>[1]apple_averages!J104</f>
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="5">
         <v>8.3889575607746236E-2</v>
       </c>
       <c r="L9" s="4">
@@ -2552,10 +2558,10 @@
       <c r="J31" s="4">
         <v>1.35E-2</v>
       </c>
-      <c r="K31" s="6">
+      <c r="K31" s="5">
         <v>-6.7293659802172279E-3</v>
       </c>
-      <c r="L31" s="6">
+      <c r="L31" s="5">
         <v>1.2485811577752415E-2</v>
       </c>
       <c r="M31" s="3" t="s">
@@ -2593,7 +2599,7 @@
       <c r="J32" s="4">
         <v>-5.6399999999999999E-2</v>
       </c>
-      <c r="K32" s="6">
+      <c r="K32" s="5">
         <v>-3.1375324368954849E-2</v>
       </c>
       <c r="L32" s="4">
@@ -2634,7 +2640,7 @@
       <c r="J33" s="4">
         <v>-1.7899999999999999E-2</v>
       </c>
-      <c r="K33" s="6">
+      <c r="K33" s="5">
         <v>7.2806424979359186E-3</v>
       </c>
       <c r="L33" s="4">
@@ -2675,7 +2681,7 @@
       <c r="J34" s="4">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="K34" s="6">
+      <c r="K34" s="5">
         <v>-1.7659963436928661E-2</v>
       </c>
       <c r="L34" s="4">
@@ -2716,7 +2722,7 @@
       <c r="J35" s="4">
         <v>0.1605</v>
       </c>
-      <c r="K35" s="6">
+      <c r="K35" s="5">
         <v>0.11111494351987572</v>
       </c>
       <c r="L35" s="4">
@@ -3700,10 +3706,10 @@
       <c r="J59" s="4">
         <v>-0.18149999999999999</v>
       </c>
-      <c r="K59" s="8">
+      <c r="K59" s="6">
         <v>-0.20607826810990837</v>
       </c>
-      <c r="L59" s="8">
+      <c r="L59" s="6">
         <v>-0.26852622814321392</v>
       </c>
       <c r="M59" s="3" t="s">
@@ -3741,10 +3747,10 @@
       <c r="J60" s="4">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="K60" s="8">
+      <c r="K60" s="6">
         <v>0.26743398781313465</v>
       </c>
-      <c r="L60" s="8">
+      <c r="L60" s="6">
         <v>0.26337169939065674</v>
       </c>
       <c r="M60" s="3" t="s">
@@ -3782,10 +3788,10 @@
       <c r="J61" s="4">
         <v>-2.12E-2</v>
       </c>
-      <c r="K61" s="8">
+      <c r="K61" s="6">
         <v>-3.0800821355236097E-2</v>
       </c>
-      <c r="L61" s="8">
+      <c r="L61" s="6">
         <v>-6.5023956194387389E-2</v>
       </c>
       <c r="M61" s="3" t="s">
@@ -3823,10 +3829,10 @@
       <c r="J62" s="4">
         <v>-1E-3</v>
       </c>
-      <c r="K62" s="8">
+      <c r="K62" s="6">
         <v>-9.5419847328237495E-4</v>
       </c>
-      <c r="L62" s="8">
+      <c r="L62" s="6">
         <v>3.8167938931297662E-2</v>
       </c>
       <c r="M62" s="3" t="s">
@@ -3864,10 +3870,10 @@
       <c r="J63" s="4">
         <v>-9.1600000000000001E-2</v>
       </c>
-      <c r="K63" s="8">
+      <c r="K63" s="6">
         <v>-8.2848837209302362E-2</v>
       </c>
-      <c r="L63" s="8">
+      <c r="L63" s="6">
         <v>-4.5784883720930147E-2</v>
       </c>
       <c r="M63" s="3" t="s">
@@ -3905,10 +3911,10 @@
       <c r="J64" s="4">
         <v>-5.5999999999999999E-3</v>
       </c>
-      <c r="K64" s="8">
+      <c r="K64" s="6">
         <v>-5.2808988764045051E-2</v>
       </c>
-      <c r="L64" s="8">
+      <c r="L64" s="6">
         <v>-2.1910112359550538E-2</v>
       </c>
       <c r="M64" s="3" t="s">
@@ -3946,10 +3952,10 @@
       <c r="J65" s="4">
         <v>0.1268</v>
       </c>
-      <c r="K65" s="8">
+      <c r="K65" s="6">
         <v>8.2118561710398552E-2</v>
       </c>
-      <c r="L65" s="8">
+      <c r="L65" s="6">
         <v>7.0942662779397425E-2</v>
       </c>
       <c r="M65" s="3" t="s">
@@ -3987,10 +3993,10 @@
       <c r="J66" s="4">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="K66" s="8">
+      <c r="K66" s="6">
         <v>9.4446543256516913E-2</v>
       </c>
-      <c r="L66" s="8">
+      <c r="L66" s="6">
         <v>8.122402720060462E-2</v>
       </c>
       <c r="M66" s="3" t="s">
@@ -4028,10 +4034,10 @@
       <c r="J67" s="4">
         <v>0.1045</v>
       </c>
-      <c r="K67" s="8">
+      <c r="K67" s="6">
         <v>0.12228887863405613</v>
       </c>
-      <c r="L67" s="8">
+      <c r="L67" s="6">
         <v>7.7526534379326328E-2</v>
       </c>
       <c r="M67" s="3" t="s">
@@ -4069,10 +4075,10 @@
       <c r="J68" s="4">
         <v>-3.6799999999999999E-2</v>
       </c>
-      <c r="K68" s="8">
+      <c r="K68" s="6">
         <v>-4.1032148900169152E-2</v>
       </c>
-      <c r="L68" s="8">
+      <c r="L68" s="6">
         <v>5.4991539763113995E-3</v>
       </c>
       <c r="M68" s="3" t="s">
@@ -4110,10 +4116,10 @@
       <c r="J69" s="4">
         <v>0.1008</v>
       </c>
-      <c r="K69" s="8">
+      <c r="K69" s="6">
         <v>0.11097230897355814</v>
       </c>
-      <c r="L69" s="8">
+      <c r="L69" s="6">
         <v>0.13220903601915479</v>
       </c>
       <c r="M69" s="3" t="s">
@@ -4151,10 +4157,10 @@
       <c r="J70" s="4">
         <v>5.8299999999999998E-2</v>
       </c>
-      <c r="K70" s="8">
+      <c r="K70" s="6">
         <v>-1.1525163273147232E-3</v>
       </c>
-      <c r="L70" s="8">
+      <c r="L70" s="6">
         <v>-4.5524394928928236E-2</v>
       </c>
       <c r="M70" s="3" t="s">
@@ -4192,10 +4198,10 @@
       <c r="J71" s="4">
         <v>-7.17E-2</v>
       </c>
-      <c r="K71" s="8">
+      <c r="K71" s="6">
         <v>-0.10541412692721408</v>
       </c>
-      <c r="L71" s="8">
+      <c r="L71" s="6">
         <v>-0.10469702402294734</v>
       </c>
       <c r="M71" s="3" t="s">
@@ -4233,10 +4239,10 @@
       <c r="J72" s="4">
         <v>5.3100000000000001E-2</v>
       </c>
-      <c r="K72" s="8">
+      <c r="K72" s="6">
         <v>6.9127896025616753E-2</v>
       </c>
-      <c r="L72" s="8">
+      <c r="L72" s="6">
         <v>6.5737427010736482E-2</v>
       </c>
       <c r="M72" s="3" t="s">
@@ -4274,10 +4280,10 @@
       <c r="J73" s="4">
         <v>4.2099999999999999E-2</v>
       </c>
-      <c r="K73" s="8">
+      <c r="K73" s="6">
         <v>4.9781659388646204E-2</v>
       </c>
-      <c r="L73" s="8">
+      <c r="L73" s="6">
         <v>3.4235807860262035E-2</v>
       </c>
       <c r="M73" s="3" t="s">
@@ -4315,10 +4321,10 @@
       <c r="J74" s="4">
         <v>2.35E-2</v>
       </c>
-      <c r="K74" s="8">
+      <c r="K74" s="6">
         <v>-1.7115294849852081E-2</v>
       </c>
-      <c r="L74" s="8">
+      <c r="L74" s="6">
         <v>-3.2674653804262155E-3</v>
       </c>
       <c r="M74" s="3" t="s">
@@ -4356,10 +4362,10 @@
       <c r="J75" s="4">
         <v>0.18210000000000001</v>
       </c>
-      <c r="K75" s="8">
+      <c r="K75" s="6">
         <v>0.17299764428739683</v>
       </c>
-      <c r="L75" s="8">
+      <c r="L75" s="6">
         <v>0.18389281507656063</v>
       </c>
       <c r="M75" s="3" t="s">
@@ -4397,10 +4403,10 @@
       <c r="J76" s="4">
         <v>0.1802</v>
       </c>
-      <c r="K76" s="8">
+      <c r="K76" s="6">
         <v>0.13624783450524824</v>
       </c>
-      <c r="L76" s="8">
+      <c r="L76" s="6">
         <v>9.1205543666564859E-2</v>
       </c>
       <c r="M76" s="3" t="s">
@@ -4438,10 +4444,10 @@
       <c r="J77" s="4">
         <v>-8.2900000000000001E-2</v>
       </c>
-      <c r="K77" s="8">
+      <c r="K77" s="6">
         <v>-0.11131270978862384</v>
       </c>
-      <c r="L77" s="8">
+      <c r="L77" s="6">
         <v>-4.0188696362151943E-2</v>
       </c>
       <c r="M77" s="3" t="s">
@@ -4479,10 +4485,10 @@
       <c r="J78" s="4">
         <v>-1.4E-3</v>
       </c>
-      <c r="K78" s="8">
+      <c r="K78" s="6">
         <v>-9.3243117990545965E-2</v>
       </c>
-      <c r="L78" s="8">
+      <c r="L78" s="6">
         <v>-0.1520066734637131</v>
       </c>
       <c r="M78" s="3" t="s">
@@ -4520,10 +4526,10 @@
       <c r="J79" s="4">
         <v>-0.12970000000000001</v>
       </c>
-      <c r="K79" s="8">
+      <c r="K79" s="6">
         <v>-0.13690036900369007</v>
       </c>
-      <c r="L79" s="8">
+      <c r="L79" s="6">
         <v>-0.14105166051660523</v>
       </c>
       <c r="M79" s="3" t="s">
@@ -4561,10 +4567,10 @@
       <c r="J80" s="4">
         <v>-0.1313</v>
       </c>
-      <c r="K80" s="8">
+      <c r="K80" s="6">
         <v>-0.1128428296731101</v>
       </c>
-      <c r="L80" s="8">
+      <c r="L80" s="6">
         <v>-4.4934723206153215E-2</v>
       </c>
       <c r="M80" s="3" t="s">
@@ -4602,10 +4608,10 @@
       <c r="J81" s="4">
         <v>0.1903</v>
       </c>
-      <c r="K81" s="8">
+      <c r="K81" s="6">
         <v>0.27585170340681375</v>
       </c>
-      <c r="L81" s="8">
+      <c r="L81" s="6">
         <v>0.25120240480961931</v>
       </c>
       <c r="M81" s="3" t="s">
@@ -4643,10 +4649,10 @@
       <c r="J82" s="4">
         <v>3.8600000000000002E-2</v>
       </c>
-      <c r="K82" s="8">
+      <c r="K82" s="6">
         <v>4.6975836710190677E-2</v>
       </c>
-      <c r="L82" s="8">
+      <c r="L82" s="6">
         <v>5.6431037070388879E-2</v>
       </c>
       <c r="M82" s="3" t="s">
@@ -4684,10 +4690,10 @@
       <c r="J83" s="4">
         <v>-7.3999999999999996E-2</v>
       </c>
-      <c r="K83" s="8">
+      <c r="K83" s="6">
         <v>-5.3357047576700678E-2</v>
       </c>
-      <c r="L83" s="8">
+      <c r="L83" s="6">
         <v>-7.1142730102267571E-2</v>
       </c>
       <c r="M83" s="3" t="s">
@@ -4725,10 +4731,10 @@
       <c r="J84" s="4">
         <v>0.1237</v>
       </c>
-      <c r="K84" s="8">
+      <c r="K84" s="6">
         <v>0.15012224938875307</v>
       </c>
-      <c r="L84" s="8">
+      <c r="L84" s="6">
         <v>8.3618581907090483E-2</v>
       </c>
       <c r="M84" s="3" t="s">
@@ -4766,10 +4772,10 @@
       <c r="J85" s="4">
         <v>0.1386</v>
       </c>
-      <c r="K85" s="8">
+      <c r="K85" s="6">
         <v>9.7076867556838531E-2</v>
       </c>
-      <c r="L85" s="8">
+      <c r="L85" s="6">
         <v>0.12306026705160589</v>
       </c>
       <c r="M85" s="3" t="s">
@@ -4807,10 +4813,10 @@
       <c r="J86" s="4">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="K86" s="8">
+      <c r="K86" s="6">
         <v>0.15039768618944316</v>
       </c>
-      <c r="L86" s="8">
+      <c r="L86" s="6">
         <v>0.19088937093275482</v>
       </c>
       <c r="M86" s="3" t="s">
@@ -4848,10 +4854,10 @@
       <c r="J87" s="4">
         <v>0.15210000000000001</v>
       </c>
-      <c r="K87" s="8">
+      <c r="K87" s="6">
         <v>0.22434635929153779</v>
       </c>
-      <c r="L87" s="8">
+      <c r="L87" s="6">
         <v>0.28338487489457398</v>
       </c>
       <c r="M87" s="3" t="s">
@@ -4889,10 +4895,10 @@
       <c r="J88" s="4">
         <v>5.5899999999999998E-2</v>
       </c>
-      <c r="K88" s="8">
+      <c r="K88" s="6">
         <v>4.020100502512558E-2</v>
       </c>
-      <c r="L88" s="8">
+      <c r="L88" s="6">
         <v>3.0653266331658324E-2</v>
       </c>
       <c r="M88" s="3" t="s">
@@ -4930,10 +4936,10 @@
       <c r="J89" s="4">
         <v>0.29809999999999998</v>
       </c>
-      <c r="K89" s="8">
+      <c r="K89" s="6">
         <v>0.36328759037922387</v>
       </c>
-      <c r="L89" s="8">
+      <c r="L89" s="6">
         <v>0.38940534159657658</v>
       </c>
       <c r="M89" s="3" t="s">
@@ -4971,10 +4977,10 @@
       <c r="J90" s="4">
         <v>-2.3699999999999999E-2</v>
       </c>
-      <c r="K90" s="8">
+      <c r="K90" s="6">
         <v>-7.844990548204156E-2</v>
       </c>
-      <c r="L90" s="8">
+      <c r="L90" s="6">
         <v>-0.12820072177350061</v>
       </c>
       <c r="M90" s="3" t="s">
@@ -5012,10 +5018,10 @@
       <c r="J91" s="4">
         <v>-0.18179999999999999</v>
       </c>
-      <c r="K91" s="8">
+      <c r="K91" s="6">
         <v>-0.26674409601238858</v>
       </c>
-      <c r="L91" s="8">
+      <c r="L91" s="6">
         <v>-0.27777777777777768</v>
       </c>
       <c r="M91" s="3" t="s">
@@ -5053,10 +5059,10 @@
       <c r="J92" s="4">
         <v>-0.14499999999999999</v>
       </c>
-      <c r="K92" s="8">
+      <c r="K92" s="6">
         <v>-0.19704433497536944</v>
       </c>
-      <c r="L92" s="8">
+      <c r="L92" s="6">
         <v>-0.18938149972632723</v>
       </c>
       <c r="M92" s="3" t="s">
@@ -5094,10 +5100,10 @@
       <c r="J93" s="4">
         <v>-1.4999999999999999E-2</v>
       </c>
-      <c r="K93" s="8">
+      <c r="K93" s="6">
         <v>-7.0516911295469109E-2</v>
       </c>
-      <c r="L93" s="8">
+      <c r="L93" s="6">
         <v>-0.13688576898532223</v>
       </c>
       <c r="M93" s="3" t="s">
@@ -5135,10 +5141,10 @@
       <c r="J94" s="4">
         <v>-4.4699999999999997E-2</v>
       </c>
-      <c r="K94" s="8">
+      <c r="K94" s="6">
         <v>0.2303070761014685</v>
       </c>
-      <c r="L94" s="8">
+      <c r="L94" s="6">
         <v>0.17423230974632831</v>
       </c>
       <c r="M94" s="3" t="s">
@@ -5176,10 +5182,10 @@
       <c r="J95" s="4">
         <v>-0.1628</v>
       </c>
-      <c r="K95" s="8">
+      <c r="K95" s="6">
         <v>-0.21070422535211264</v>
       </c>
-      <c r="L95" s="8">
+      <c r="L95" s="6">
         <v>-0.17577464788732389</v>
       </c>
       <c r="M95" s="3" t="s">
@@ -5217,17 +5223,17 @@
       <c r="J96" s="4">
         <v>-0.14530000000000001</v>
       </c>
-      <c r="K96" s="8">
+      <c r="K96" s="6">
         <v>-0.1100271002710026</v>
       </c>
-      <c r="L96" s="8">
+      <c r="L96" s="6">
         <v>1.2466124661246747E-2</v>
       </c>
       <c r="M96" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="97" spans="1:14" s="3" customFormat="1">
+    <row r="97" spans="1:13" s="3" customFormat="1">
       <c r="A97" s="2">
         <v>42669</v>
       </c>
@@ -5258,17 +5264,17 @@
       <c r="J97" s="4">
         <v>6.4000000000000003E-3</v>
       </c>
-      <c r="K97" s="8">
+      <c r="K97" s="6">
         <v>1.8507807981492208E-2</v>
       </c>
-      <c r="L97" s="8">
+      <c r="L97" s="6">
         <v>0.10641989589358003</v>
       </c>
       <c r="M97" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="98" spans="1:14" s="3" customFormat="1">
+    <row r="98" spans="1:13" s="3" customFormat="1">
       <c r="A98" s="2">
         <v>42774</v>
       </c>
@@ -5299,31 +5305,92 @@
       <c r="J98" s="4">
         <v>-0.1234</v>
       </c>
-      <c r="K98" s="8">
+      <c r="K98" s="6">
         <v>-0.10576923076923084</v>
       </c>
-      <c r="L98" s="8">
+      <c r="L98" s="6">
         <v>-0.14369658119658113</v>
       </c>
       <c r="M98" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:14" s="5" customFormat="1">
-      <c r="K99" s="7"/>
-      <c r="L99" s="7"/>
-      <c r="N99" s="5" t="s">
+    <row r="99" spans="1:13" s="7" customFormat="1">
+      <c r="A99" s="8">
+        <v>42059</v>
+      </c>
+      <c r="K99" s="4"/>
+      <c r="L99" s="4"/>
+      <c r="M99" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="100" spans="1:14">
+    <row r="100" spans="1:13">
+      <c r="A100" s="1">
+        <v>42145</v>
+      </c>
       <c r="K100"/>
-    </row>
-    <row r="101" spans="1:14">
+      <c r="M100" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13">
+      <c r="A101" s="1">
+        <v>42236</v>
+      </c>
       <c r="K101"/>
-    </row>
-    <row r="102" spans="1:14">
+      <c r="M101" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13">
+      <c r="A102" s="1">
+        <v>42332</v>
+      </c>
       <c r="K102"/>
+      <c r="M102" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13">
+      <c r="A103" s="1">
+        <v>42424</v>
+      </c>
+      <c r="M103" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13">
+      <c r="A104" s="1">
+        <v>42515</v>
+      </c>
+      <c r="M104" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13">
+      <c r="A105" s="1">
+        <v>42606</v>
+      </c>
+      <c r="M105" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13">
+      <c r="A106" s="1">
+        <v>42696</v>
+      </c>
+      <c r="M106" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13">
+      <c r="A107" s="1">
+        <v>42788</v>
+      </c>
+      <c r="M107" s="7" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added hp averages for mitesh
</commit_message>
<xml_diff>
--- a/data/general/all_averages.xlsx
+++ b/data/general/all_averages.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ldona\Desktop\data_project\fund\data\general\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="3480" yWindow="0" windowWidth="25080" windowHeight="17540"/>
   </bookViews>
@@ -12,13 +17,13 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -108,7 +113,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -623,7 +628,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="apple_averages"/>
@@ -1188,7 +1193,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1198,26 +1203,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="E102" sqref="E102"/>
+    <sheetView tabSelected="1" topLeftCell="F95" workbookViewId="0">
+      <selection activeCell="I102" sqref="I102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" customWidth="1"/>
-    <col min="5" max="5" width="16.5" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" customWidth="1"/>
-    <col min="8" max="9" width="14.6640625" customWidth="1"/>
-    <col min="10" max="10" width="8.5" customWidth="1"/>
-    <col min="11" max="11" width="20.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.5" style="5" customWidth="1"/>
+    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" customWidth="1"/>
+    <col min="3" max="3" width="13.6328125" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" customWidth="1"/>
+    <col min="7" max="7" width="15.6328125" customWidth="1"/>
+    <col min="8" max="9" width="14.6328125" customWidth="1"/>
+    <col min="10" max="10" width="8.453125" customWidth="1"/>
+    <col min="11" max="11" width="20.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.453125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1258,7 +1263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <f>[1]apple_averages!A12</f>
         <v>42123</v>
@@ -1309,7 +1314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <f>[1]apple_averages!A24</f>
         <v>42207</v>
@@ -1360,7 +1365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <f>[1]apple_averages!A38</f>
         <v>42305</v>
@@ -1411,7 +1416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <f>[1]apple_averages!A51</f>
         <v>42396</v>
@@ -1462,7 +1467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <f>[1]apple_averages!A64</f>
         <v>42487</v>
@@ -1513,7 +1518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <f>[1]apple_averages!A77</f>
         <v>42578</v>
@@ -1564,7 +1569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <f>[1]apple_averages!A90</f>
         <v>42669</v>
@@ -1615,7 +1620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <f>[1]apple_averages!A104</f>
         <v>42767</v>
@@ -1666,7 +1671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="3" customFormat="1">
+    <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>42116</v>
       </c>
@@ -1707,7 +1712,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="3" customFormat="1">
+    <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>42207</v>
       </c>
@@ -1748,7 +1753,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="3" customFormat="1">
+    <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>42298</v>
       </c>
@@ -1789,7 +1794,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="3" customFormat="1">
+    <row r="13" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>42396</v>
       </c>
@@ -1830,7 +1835,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="3" customFormat="1">
+    <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>42487</v>
       </c>
@@ -1871,7 +1876,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="3" customFormat="1">
+    <row r="15" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>42578</v>
       </c>
@@ -1912,7 +1917,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="3" customFormat="1">
+    <row r="16" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>42669</v>
       </c>
@@ -1953,7 +1958,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="3" customFormat="1">
+    <row r="17" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>42767</v>
       </c>
@@ -1994,7 +1999,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="3" customFormat="1">
+    <row r="18" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>42109</v>
       </c>
@@ -2035,7 +2040,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="3" customFormat="1">
+    <row r="19" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>42199</v>
       </c>
@@ -2076,7 +2081,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="3" customFormat="1">
+    <row r="20" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>42291</v>
       </c>
@@ -2117,7 +2122,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="3" customFormat="1">
+    <row r="21" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>42383</v>
       </c>
@@ -2158,7 +2163,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="3" customFormat="1">
+    <row r="22" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>42480</v>
       </c>
@@ -2199,7 +2204,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="3" customFormat="1">
+    <row r="23" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>42571</v>
       </c>
@@ -2240,7 +2245,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="3" customFormat="1">
+    <row r="24" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>42657</v>
       </c>
@@ -2281,7 +2286,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="3" customFormat="1">
+    <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>42765</v>
       </c>
@@ -2322,7 +2327,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="3" customFormat="1">
+    <row r="26" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>42116</v>
       </c>
@@ -2363,7 +2368,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="3" customFormat="1">
+    <row r="27" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>42214</v>
       </c>
@@ -2404,7 +2409,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="3" customFormat="1">
+    <row r="28" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>42312</v>
       </c>
@@ -2445,7 +2450,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="3" customFormat="1">
+    <row r="29" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>42396</v>
       </c>
@@ -2486,7 +2491,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="3" customFormat="1">
+    <row r="30" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>42487</v>
       </c>
@@ -2527,7 +2532,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="3" customFormat="1">
+    <row r="31" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>42578</v>
       </c>
@@ -2568,7 +2573,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:13" s="3" customFormat="1">
+    <row r="32" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>42676</v>
       </c>
@@ -2609,7 +2614,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="3" customFormat="1">
+    <row r="33" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>42767</v>
       </c>
@@ -2650,7 +2655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="3" customFormat="1">
+    <row r="34" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>42116</v>
       </c>
@@ -2691,7 +2696,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="3" customFormat="1">
+    <row r="35" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>42200</v>
       </c>
@@ -2732,7 +2737,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="3" customFormat="1">
+    <row r="36" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>42298</v>
       </c>
@@ -2773,7 +2778,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:13" s="3" customFormat="1">
+    <row r="37" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>42396</v>
       </c>
@@ -2814,7 +2819,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:13" s="3" customFormat="1">
+    <row r="38" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>42480</v>
       </c>
@@ -2855,7 +2860,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:13" s="3" customFormat="1">
+    <row r="39" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>42578</v>
       </c>
@@ -2896,7 +2901,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="3" customFormat="1">
+    <row r="40" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>42669</v>
       </c>
@@ -2937,7 +2942,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:13" s="3" customFormat="1">
+    <row r="41" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>42760</v>
       </c>
@@ -2978,7 +2983,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:13" s="3" customFormat="1">
+    <row r="42" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>42109</v>
       </c>
@@ -3019,7 +3024,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:13" s="3" customFormat="1">
+    <row r="43" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>42200</v>
       </c>
@@ -3060,7 +3065,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="3" customFormat="1">
+    <row r="44" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>42291</v>
       </c>
@@ -3101,7 +3106,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:13" s="3" customFormat="1">
+    <row r="45" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>42382</v>
       </c>
@@ -3142,7 +3147,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:13" s="3" customFormat="1">
+    <row r="46" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>42473</v>
       </c>
@@ -3183,7 +3188,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:13" s="3" customFormat="1">
+    <row r="47" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>42564</v>
       </c>
@@ -3224,7 +3229,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:13" s="3" customFormat="1">
+    <row r="48" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>42655</v>
       </c>
@@ -3265,7 +3270,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:13" s="3" customFormat="1">
+    <row r="49" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>42753</v>
       </c>
@@ -3306,7 +3311,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:13" s="3" customFormat="1">
+    <row r="50" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>42102</v>
       </c>
@@ -3347,7 +3352,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:13" s="3" customFormat="1">
+    <row r="51" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>42200</v>
       </c>
@@ -3388,7 +3393,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:13" s="3" customFormat="1">
+    <row r="52" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>42284</v>
       </c>
@@ -3429,7 +3434,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:13" s="3" customFormat="1">
+    <row r="53" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>42382</v>
       </c>
@@ -3470,7 +3475,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:13" s="3" customFormat="1">
+    <row r="54" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>42473</v>
       </c>
@@ -3511,7 +3516,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:13" s="3" customFormat="1">
+    <row r="55" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>42571</v>
       </c>
@@ -3552,7 +3557,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:13" s="3" customFormat="1">
+    <row r="56" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>42655</v>
       </c>
@@ -3593,7 +3598,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:13" s="3" customFormat="1">
+    <row r="57" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>42760</v>
       </c>
@@ -3634,7 +3639,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:13" s="3" customFormat="1">
+    <row r="58" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>42095</v>
       </c>
@@ -3675,7 +3680,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:13" s="3" customFormat="1">
+    <row r="59" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>42174</v>
       </c>
@@ -3716,7 +3721,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:13" s="3" customFormat="1">
+    <row r="60" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>42273</v>
       </c>
@@ -3757,7 +3762,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:13" s="3" customFormat="1">
+    <row r="61" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>42359</v>
       </c>
@@ -3798,7 +3803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:13" s="3" customFormat="1">
+    <row r="62" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>42458</v>
       </c>
@@ -3839,7 +3844,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:13" s="3" customFormat="1">
+    <row r="63" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>42549</v>
       </c>
@@ -3880,7 +3885,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:13" s="3" customFormat="1">
+    <row r="64" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
         <v>42641</v>
       </c>
@@ -3921,7 +3926,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:13" s="3" customFormat="1">
+    <row r="65" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>42725</v>
       </c>
@@ -3962,7 +3967,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:13" s="3" customFormat="1">
+    <row r="66" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
         <v>42816</v>
       </c>
@@ -4003,7 +4008,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:13" s="3" customFormat="1">
+    <row r="67" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
         <v>42116</v>
       </c>
@@ -4044,7 +4049,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:13" s="3" customFormat="1">
+    <row r="68" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
         <v>42200</v>
       </c>
@@ -4085,7 +4090,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:13" s="3" customFormat="1">
+    <row r="69" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>42298</v>
       </c>
@@ -4126,7 +4131,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:13" s="3" customFormat="1">
+    <row r="70" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>42396</v>
       </c>
@@ -4167,7 +4172,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:13" s="3" customFormat="1">
+    <row r="71" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>42480</v>
       </c>
@@ -4208,7 +4213,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:13" s="3" customFormat="1">
+    <row r="72" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
         <v>42564</v>
       </c>
@@ -4249,7 +4254,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:13" s="3" customFormat="1">
+    <row r="73" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
         <v>42662</v>
       </c>
@@ -4290,7 +4295,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:13" s="3" customFormat="1">
+    <row r="74" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>42760</v>
       </c>
@@ -4331,7 +4336,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:13" s="3" customFormat="1">
+    <row r="75" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
         <v>42109</v>
       </c>
@@ -4372,7 +4377,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:13" s="3" customFormat="1">
+    <row r="76" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>42200</v>
       </c>
@@ -4413,7 +4418,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:13" s="3" customFormat="1">
+    <row r="77" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>42291</v>
       </c>
@@ -4454,7 +4459,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:13" s="3" customFormat="1">
+    <row r="78" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
         <v>42382</v>
       </c>
@@ -4495,7 +4500,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:13" s="3" customFormat="1">
+    <row r="79" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>42473</v>
       </c>
@@ -4536,7 +4541,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="80" spans="1:13" s="3" customFormat="1">
+    <row r="80" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>42564</v>
       </c>
@@ -4577,7 +4582,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:13" s="3" customFormat="1">
+    <row r="81" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>42655</v>
       </c>
@@ -4618,7 +4623,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:13" s="3" customFormat="1">
+    <row r="82" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A82" s="2">
         <v>42753</v>
       </c>
@@ -4659,7 +4664,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="1:13" s="3" customFormat="1">
+    <row r="83" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A83" s="2">
         <v>42130</v>
       </c>
@@ -4700,7 +4705,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:13" s="3" customFormat="1">
+    <row r="84" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A84" s="2">
         <v>42221</v>
       </c>
@@ -4741,7 +4746,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:13" s="3" customFormat="1">
+    <row r="85" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
         <v>42307</v>
       </c>
@@ -4782,7 +4787,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:13" s="3" customFormat="1">
+    <row r="86" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A86" s="2">
         <v>42412</v>
       </c>
@@ -4823,7 +4828,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:13" s="3" customFormat="1">
+    <row r="87" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A87" s="2">
         <v>42496</v>
       </c>
@@ -4864,7 +4869,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:13" s="3" customFormat="1">
+    <row r="88" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A88" s="2">
         <v>42587</v>
       </c>
@@ -4905,7 +4910,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:13" s="3" customFormat="1">
+    <row r="89" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A89" s="2">
         <v>42678</v>
       </c>
@@ -4946,7 +4951,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:13" s="3" customFormat="1">
+    <row r="90" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A90" s="2">
         <v>42769</v>
       </c>
@@ -4987,7 +4992,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:13" s="3" customFormat="1">
+    <row r="91" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A91" s="2">
         <v>42116</v>
       </c>
@@ -5028,7 +5033,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="92" spans="1:13" s="3" customFormat="1">
+    <row r="92" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A92" s="2">
         <v>42207</v>
       </c>
@@ -5069,7 +5074,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:13" s="3" customFormat="1">
+    <row r="93" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A93" s="2">
         <v>42298</v>
       </c>
@@ -5110,7 +5115,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="94" spans="1:13" s="3" customFormat="1">
+    <row r="94" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A94" s="2">
         <v>42410</v>
       </c>
@@ -5151,7 +5156,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="95" spans="1:13" s="3" customFormat="1">
+    <row r="95" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A95" s="2">
         <v>42480</v>
       </c>
@@ -5192,7 +5197,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="96" spans="1:13" s="3" customFormat="1">
+    <row r="96" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A96" s="2">
         <v>42571</v>
       </c>
@@ -5233,7 +5238,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="97" spans="1:13" s="3" customFormat="1">
+    <row r="97" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A97" s="2">
         <v>42669</v>
       </c>
@@ -5274,7 +5279,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="98" spans="1:13" s="3" customFormat="1">
+    <row r="98" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A98" s="2">
         <v>42774</v>
       </c>
@@ -5315,78 +5320,370 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:13" s="7" customFormat="1">
+    <row r="99" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A99" s="8">
         <v>42059</v>
       </c>
-      <c r="K99" s="4"/>
-      <c r="L99" s="4"/>
+      <c r="B99" s="7">
+        <v>0.26258889770312399</v>
+      </c>
+      <c r="C99" s="7">
+        <v>0.26258889770312399</v>
+      </c>
+      <c r="D99" s="7">
+        <v>0.26258889770312399</v>
+      </c>
+      <c r="E99" s="7">
+        <v>0.26258889770312399</v>
+      </c>
+      <c r="F99" s="7">
+        <v>-8.9457002296876031E-2</v>
+      </c>
+      <c r="G99" s="7">
+        <v>-8.9457002296876031E-2</v>
+      </c>
+      <c r="H99" s="7">
+        <v>-8.9457002296876031E-2</v>
+      </c>
+      <c r="I99" s="7">
+        <v>-8.9457002296876031E-2</v>
+      </c>
+      <c r="J99" s="6">
+        <v>-9.9199999999999997E-2</v>
+      </c>
+      <c r="K99" s="6">
+        <v>-0.1018</v>
+      </c>
+      <c r="L99" s="6">
+        <v>-0.1512</v>
+      </c>
       <c r="M99" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="100" spans="1:13">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>42145</v>
       </c>
-      <c r="K100"/>
+      <c r="B100">
+        <v>0.30768564305909002</v>
+      </c>
+      <c r="C100">
+        <v>0.45363239782779052</v>
+      </c>
+      <c r="D100">
+        <v>-4.3410709576104559E-2</v>
+      </c>
+      <c r="E100">
+        <v>-0.14094715878829592</v>
+      </c>
+      <c r="F100">
+        <v>-4.4360256940910003E-2</v>
+      </c>
+      <c r="G100">
+        <v>0.1015864978277905</v>
+      </c>
+      <c r="H100">
+        <v>-0.39545660957610457</v>
+      </c>
+      <c r="I100">
+        <v>-0.49299305878829591</v>
+      </c>
+      <c r="J100" s="6">
+        <v>2.75E-2</v>
+      </c>
+      <c r="K100" s="6">
+        <v>-1.2699999999999999E-2</v>
+      </c>
+      <c r="L100" s="6">
+        <v>-2.69E-2</v>
+      </c>
       <c r="M100" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="101" spans="1:13">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>42236</v>
       </c>
-      <c r="K101"/>
+      <c r="B101">
+        <v>-0.55891422509505695</v>
+      </c>
+      <c r="C101">
+        <v>-4.9268461399641472E-2</v>
+      </c>
+      <c r="D101">
+        <v>0.20244984190642928</v>
+      </c>
+      <c r="E101">
+        <v>0.40801088718464446</v>
+      </c>
+      <c r="F101">
+        <v>-0.91096012509505697</v>
+      </c>
+      <c r="G101">
+        <v>-0.40131436139964149</v>
+      </c>
+      <c r="H101">
+        <v>-0.14959605809357074</v>
+      </c>
+      <c r="I101">
+        <v>5.5964987184644432E-2</v>
+      </c>
+      <c r="J101" s="6">
+        <v>4.4000000000000003E-3</v>
+      </c>
+      <c r="K101" s="6">
+        <v>1.61E-2</v>
+      </c>
+      <c r="L101" s="6">
+        <v>2.8500000000000001E-2</v>
+      </c>
       <c r="M101" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="102" spans="1:13">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>42332</v>
       </c>
-      <c r="K102"/>
+      <c r="B102">
+        <v>1.06160778568571</v>
+      </c>
+      <c r="C102">
+        <v>1.3256068844950251</v>
+      </c>
+      <c r="D102">
+        <v>0.86341328638264492</v>
+      </c>
+      <c r="E102">
+        <v>0.58186138475597937</v>
+      </c>
+      <c r="F102">
+        <v>0.70956188568570999</v>
+      </c>
+      <c r="G102">
+        <v>0.97356098449502504</v>
+      </c>
+      <c r="H102">
+        <v>0.5113673863826449</v>
+      </c>
+      <c r="I102">
+        <v>0.22981548475597935</v>
+      </c>
+      <c r="J102" s="6">
+        <v>-0.1366</v>
+      </c>
+      <c r="K102" s="6">
+        <v>-0.1837</v>
+      </c>
+      <c r="L102" s="6">
+        <v>-0.17280000000000001</v>
+      </c>
       <c r="M102" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="103" spans="1:13">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>42424</v>
       </c>
+      <c r="B103">
+        <v>1.4801167358532099</v>
+      </c>
+      <c r="C103">
+        <v>0.95323144319446196</v>
+      </c>
+      <c r="D103">
+        <v>1.274004333557853</v>
+      </c>
+      <c r="E103">
+        <v>1.5622922568039723</v>
+      </c>
+      <c r="F103">
+        <v>1.1280708358532099</v>
+      </c>
+      <c r="G103">
+        <v>0.60118554319446194</v>
+      </c>
+      <c r="H103">
+        <v>0.92195843355785301</v>
+      </c>
+      <c r="I103">
+        <v>1.2102463568039723</v>
+      </c>
+      <c r="J103" s="6">
+        <v>-4.4400000000000002E-2</v>
+      </c>
+      <c r="K103" s="6">
+        <v>7.4000000000000003E-3</v>
+      </c>
+      <c r="L103" s="6">
+        <v>4.99E-2</v>
+      </c>
       <c r="M103" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="104" spans="1:13">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>42515</v>
       </c>
+      <c r="B104">
+        <v>0.100087797997142</v>
+      </c>
+      <c r="C104">
+        <v>1.0746437468217409</v>
+      </c>
+      <c r="D104">
+        <v>1.5111433938142054</v>
+      </c>
+      <c r="E104">
+        <v>1.5962436551362875</v>
+      </c>
+      <c r="F104">
+        <v>-0.25195810200285801</v>
+      </c>
+      <c r="G104">
+        <v>0.72259784682174089</v>
+      </c>
+      <c r="H104">
+        <v>1.1590974938142053</v>
+      </c>
+      <c r="I104">
+        <v>1.2441977551362875</v>
+      </c>
+      <c r="J104" s="6">
+        <v>6.8900000000000003E-2</v>
+      </c>
+      <c r="K104" s="6">
+        <v>0.10979999999999999</v>
+      </c>
+      <c r="L104" s="6">
+        <v>0.13439999999999999</v>
+      </c>
       <c r="M104" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="105" spans="1:13">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>42606</v>
       </c>
+      <c r="B105">
+        <v>0.45895248057599902</v>
+      </c>
+      <c r="C105">
+        <v>1.0268266783594244</v>
+      </c>
+      <c r="D105">
+        <v>0.80985809210870385</v>
+      </c>
+      <c r="E105">
+        <v>0.58833533175182517</v>
+      </c>
+      <c r="F105">
+        <v>0.106906580575999</v>
+      </c>
+      <c r="G105">
+        <v>0.6747807783594244</v>
+      </c>
+      <c r="H105">
+        <v>0.45781219210870383</v>
+      </c>
+      <c r="I105">
+        <v>0.23628943175182515</v>
+      </c>
+      <c r="J105" s="6">
+        <v>-2.0999999999999999E-3</v>
+      </c>
+      <c r="K105" s="6">
+        <v>-2.0999999999999999E-3</v>
+      </c>
+      <c r="L105" s="6">
+        <v>1.6E-2</v>
+      </c>
       <c r="M105" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="106" spans="1:13">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>42696</v>
       </c>
+      <c r="B106">
+        <v>0.69985791510491802</v>
+      </c>
+      <c r="C106">
+        <v>0.87507514293148903</v>
+      </c>
+      <c r="D106">
+        <v>0.49332853646079949</v>
+      </c>
+      <c r="E106">
+        <v>0.50686666673022451</v>
+      </c>
+      <c r="F106">
+        <v>0.34781201510491799</v>
+      </c>
+      <c r="G106">
+        <v>0.523029242931489</v>
+      </c>
+      <c r="H106">
+        <v>0.14128263646079947</v>
+      </c>
+      <c r="I106">
+        <v>0.15482076673022449</v>
+      </c>
+      <c r="J106" s="6">
+        <v>-6.7699999999999996E-2</v>
+      </c>
+      <c r="K106" s="6">
+        <v>-3.4500000000000003E-2</v>
+      </c>
+      <c r="L106" s="6">
+        <v>1.2500000000000001E-2</v>
+      </c>
       <c r="M106" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="107" spans="1:13">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>42788</v>
+      </c>
+      <c r="B107">
+        <v>1.8398891555974</v>
+      </c>
+      <c r="C107">
+        <v>1.2650120752743095</v>
+      </c>
+      <c r="D107">
+        <v>0.64733974601723576</v>
+      </c>
+      <c r="E107">
+        <v>0.92731852656942271</v>
+      </c>
+      <c r="F107">
+        <v>1.4878432555973999</v>
+      </c>
+      <c r="G107">
+        <v>0.91296617527430945</v>
+      </c>
+      <c r="H107">
+        <v>0.29529384601723574</v>
+      </c>
+      <c r="I107">
+        <v>0.57527262656942268</v>
+      </c>
+      <c r="J107" s="6">
+        <v>-6.7699999999999996E-2</v>
+      </c>
+      <c r="K107" s="6">
+        <v>-3.4500000000000003E-2</v>
+      </c>
+      <c r="L107" s="6">
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="M107" s="7" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
updated hp data point
</commit_message>
<xml_diff>
--- a/data/general/all_averages.xlsx
+++ b/data/general/all_averages.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ldona\Desktop\data_project\fund\data\general\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="3480" yWindow="0" windowWidth="25080" windowHeight="17540"/>
   </bookViews>
@@ -17,13 +12,13 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -113,7 +108,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -163,7 +158,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="218">
+  <cellStyleXfs count="222">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -382,19 +377,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="218">
+  <cellStyles count="222">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -503,6 +501,8 @@
     <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -611,6 +611,8 @@
     <cellStyle name="Hyperlink" xfId="212" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="214" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="216" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="218" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="220" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -628,7 +630,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="apple_averages"/>
@@ -1193,7 +1195,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1203,26 +1205,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F95" workbookViewId="0">
-      <selection activeCell="I102" sqref="I102"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.453125" customWidth="1"/>
-    <col min="3" max="3" width="13.6328125" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" customWidth="1"/>
-    <col min="5" max="5" width="16.453125" customWidth="1"/>
-    <col min="6" max="6" width="14.81640625" customWidth="1"/>
-    <col min="7" max="7" width="15.6328125" customWidth="1"/>
-    <col min="8" max="9" width="14.6328125" customWidth="1"/>
-    <col min="10" max="10" width="8.453125" customWidth="1"/>
-    <col min="11" max="11" width="20.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.453125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="5" max="5" width="16.5" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="9" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="8.5" style="5" customWidth="1"/>
+    <col min="11" max="11" width="20.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.5" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1250,7 +1252,7 @@
       <c r="I1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="5" t="s">
         <v>23</v>
       </c>
       <c r="K1" s="5" t="s">
@@ -1263,7 +1265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13">
       <c r="A2" s="1">
         <f>[1]apple_averages!A12</f>
         <v>42123</v>
@@ -1314,7 +1316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13">
       <c r="A3" s="1">
         <f>[1]apple_averages!A24</f>
         <v>42207</v>
@@ -1365,7 +1367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13">
       <c r="A4" s="1">
         <f>[1]apple_averages!A38</f>
         <v>42305</v>
@@ -1416,7 +1418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13">
       <c r="A5" s="1">
         <f>[1]apple_averages!A51</f>
         <v>42396</v>
@@ -1467,7 +1469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13">
       <c r="A6" s="1">
         <f>[1]apple_averages!A64</f>
         <v>42487</v>
@@ -1518,7 +1520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13">
       <c r="A7" s="1">
         <f>[1]apple_averages!A77</f>
         <v>42578</v>
@@ -1569,7 +1571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13">
       <c r="A8" s="1">
         <f>[1]apple_averages!A90</f>
         <v>42669</v>
@@ -1620,7 +1622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13">
       <c r="A9" s="1">
         <f>[1]apple_averages!A104</f>
         <v>42767</v>
@@ -1671,7 +1673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" s="3" customFormat="1">
       <c r="A10" s="2">
         <v>42116</v>
       </c>
@@ -1712,7 +1714,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" s="3" customFormat="1">
       <c r="A11" s="2">
         <v>42207</v>
       </c>
@@ -1753,7 +1755,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" s="3" customFormat="1">
       <c r="A12" s="2">
         <v>42298</v>
       </c>
@@ -1794,7 +1796,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" s="3" customFormat="1">
       <c r="A13" s="2">
         <v>42396</v>
       </c>
@@ -1835,7 +1837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" s="3" customFormat="1">
       <c r="A14" s="2">
         <v>42487</v>
       </c>
@@ -1876,7 +1878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" s="3" customFormat="1">
       <c r="A15" s="2">
         <v>42578</v>
       </c>
@@ -1917,7 +1919,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" s="3" customFormat="1">
       <c r="A16" s="2">
         <v>42669</v>
       </c>
@@ -1958,7 +1960,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" s="3" customFormat="1">
       <c r="A17" s="2">
         <v>42767</v>
       </c>
@@ -1999,7 +2001,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" s="3" customFormat="1">
       <c r="A18" s="2">
         <v>42109</v>
       </c>
@@ -2040,7 +2042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" s="3" customFormat="1">
       <c r="A19" s="2">
         <v>42199</v>
       </c>
@@ -2081,7 +2083,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" s="3" customFormat="1">
       <c r="A20" s="2">
         <v>42291</v>
       </c>
@@ -2122,7 +2124,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" s="3" customFormat="1">
       <c r="A21" s="2">
         <v>42383</v>
       </c>
@@ -2163,7 +2165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" s="3" customFormat="1">
       <c r="A22" s="2">
         <v>42480</v>
       </c>
@@ -2204,7 +2206,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" s="3" customFormat="1">
       <c r="A23" s="2">
         <v>42571</v>
       </c>
@@ -2245,7 +2247,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" s="3" customFormat="1">
       <c r="A24" s="2">
         <v>42657</v>
       </c>
@@ -2286,7 +2288,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" s="3" customFormat="1">
       <c r="A25" s="2">
         <v>42765</v>
       </c>
@@ -2327,7 +2329,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" s="3" customFormat="1">
       <c r="A26" s="2">
         <v>42116</v>
       </c>
@@ -2368,7 +2370,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" s="3" customFormat="1">
       <c r="A27" s="2">
         <v>42214</v>
       </c>
@@ -2409,7 +2411,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" s="3" customFormat="1">
       <c r="A28" s="2">
         <v>42312</v>
       </c>
@@ -2450,7 +2452,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" s="3" customFormat="1">
       <c r="A29" s="2">
         <v>42396</v>
       </c>
@@ -2491,7 +2493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" s="3" customFormat="1">
       <c r="A30" s="2">
         <v>42487</v>
       </c>
@@ -2532,7 +2534,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" s="3" customFormat="1">
       <c r="A31" s="2">
         <v>42578</v>
       </c>
@@ -2573,7 +2575,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" s="3" customFormat="1">
       <c r="A32" s="2">
         <v>42676</v>
       </c>
@@ -2614,7 +2616,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" s="3" customFormat="1">
       <c r="A33" s="2">
         <v>42767</v>
       </c>
@@ -2655,7 +2657,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" s="3" customFormat="1">
       <c r="A34" s="2">
         <v>42116</v>
       </c>
@@ -2696,7 +2698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" s="3" customFormat="1">
       <c r="A35" s="2">
         <v>42200</v>
       </c>
@@ -2737,7 +2739,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" s="3" customFormat="1">
       <c r="A36" s="2">
         <v>42298</v>
       </c>
@@ -2778,7 +2780,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" s="3" customFormat="1">
       <c r="A37" s="2">
         <v>42396</v>
       </c>
@@ -2819,7 +2821,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" s="3" customFormat="1">
       <c r="A38" s="2">
         <v>42480</v>
       </c>
@@ -2860,7 +2862,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" s="3" customFormat="1">
       <c r="A39" s="2">
         <v>42578</v>
       </c>
@@ -2901,7 +2903,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" s="3" customFormat="1">
       <c r="A40" s="2">
         <v>42669</v>
       </c>
@@ -2942,7 +2944,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" s="3" customFormat="1">
       <c r="A41" s="2">
         <v>42760</v>
       </c>
@@ -2983,7 +2985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" s="3" customFormat="1">
       <c r="A42" s="2">
         <v>42109</v>
       </c>
@@ -3024,7 +3026,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" s="3" customFormat="1">
       <c r="A43" s="2">
         <v>42200</v>
       </c>
@@ -3065,7 +3067,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" s="3" customFormat="1">
       <c r="A44" s="2">
         <v>42291</v>
       </c>
@@ -3106,7 +3108,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" s="3" customFormat="1">
       <c r="A45" s="2">
         <v>42382</v>
       </c>
@@ -3147,7 +3149,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" s="3" customFormat="1">
       <c r="A46" s="2">
         <v>42473</v>
       </c>
@@ -3188,7 +3190,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" s="3" customFormat="1">
       <c r="A47" s="2">
         <v>42564</v>
       </c>
@@ -3229,7 +3231,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" s="3" customFormat="1">
       <c r="A48" s="2">
         <v>42655</v>
       </c>
@@ -3270,7 +3272,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" s="3" customFormat="1">
       <c r="A49" s="2">
         <v>42753</v>
       </c>
@@ -3311,7 +3313,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" s="3" customFormat="1">
       <c r="A50" s="2">
         <v>42102</v>
       </c>
@@ -3352,7 +3354,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" s="3" customFormat="1">
       <c r="A51" s="2">
         <v>42200</v>
       </c>
@@ -3393,7 +3395,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" s="3" customFormat="1">
       <c r="A52" s="2">
         <v>42284</v>
       </c>
@@ -3434,7 +3436,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" s="3" customFormat="1">
       <c r="A53" s="2">
         <v>42382</v>
       </c>
@@ -3475,7 +3477,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" s="3" customFormat="1">
       <c r="A54" s="2">
         <v>42473</v>
       </c>
@@ -3516,7 +3518,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" s="3" customFormat="1">
       <c r="A55" s="2">
         <v>42571</v>
       </c>
@@ -3557,7 +3559,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" s="3" customFormat="1">
       <c r="A56" s="2">
         <v>42655</v>
       </c>
@@ -3598,7 +3600,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" s="3" customFormat="1">
       <c r="A57" s="2">
         <v>42760</v>
       </c>
@@ -3639,7 +3641,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" s="3" customFormat="1">
       <c r="A58" s="2">
         <v>42095</v>
       </c>
@@ -3680,7 +3682,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" s="3" customFormat="1">
       <c r="A59" s="2">
         <v>42174</v>
       </c>
@@ -3711,17 +3713,17 @@
       <c r="J59" s="4">
         <v>-0.18149999999999999</v>
       </c>
-      <c r="K59" s="6">
+      <c r="K59" s="5">
         <v>-0.20607826810990837</v>
       </c>
-      <c r="L59" s="6">
+      <c r="L59" s="5">
         <v>-0.26852622814321392</v>
       </c>
       <c r="M59" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" s="3" customFormat="1">
       <c r="A60" s="2">
         <v>42273</v>
       </c>
@@ -3752,17 +3754,17 @@
       <c r="J60" s="4">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="K60" s="6">
+      <c r="K60" s="5">
         <v>0.26743398781313465</v>
       </c>
-      <c r="L60" s="6">
+      <c r="L60" s="5">
         <v>0.26337169939065674</v>
       </c>
       <c r="M60" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" s="3" customFormat="1">
       <c r="A61" s="2">
         <v>42359</v>
       </c>
@@ -3793,17 +3795,17 @@
       <c r="J61" s="4">
         <v>-2.12E-2</v>
       </c>
-      <c r="K61" s="6">
+      <c r="K61" s="5">
         <v>-3.0800821355236097E-2</v>
       </c>
-      <c r="L61" s="6">
+      <c r="L61" s="5">
         <v>-6.5023956194387389E-2</v>
       </c>
       <c r="M61" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" s="3" customFormat="1">
       <c r="A62" s="2">
         <v>42458</v>
       </c>
@@ -3834,17 +3836,17 @@
       <c r="J62" s="4">
         <v>-1E-3</v>
       </c>
-      <c r="K62" s="6">
+      <c r="K62" s="5">
         <v>-9.5419847328237495E-4</v>
       </c>
-      <c r="L62" s="6">
+      <c r="L62" s="5">
         <v>3.8167938931297662E-2</v>
       </c>
       <c r="M62" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" s="3" customFormat="1">
       <c r="A63" s="2">
         <v>42549</v>
       </c>
@@ -3875,17 +3877,17 @@
       <c r="J63" s="4">
         <v>-9.1600000000000001E-2</v>
       </c>
-      <c r="K63" s="6">
+      <c r="K63" s="5">
         <v>-8.2848837209302362E-2</v>
       </c>
-      <c r="L63" s="6">
+      <c r="L63" s="5">
         <v>-4.5784883720930147E-2</v>
       </c>
       <c r="M63" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" s="3" customFormat="1">
       <c r="A64" s="2">
         <v>42641</v>
       </c>
@@ -3916,17 +3918,17 @@
       <c r="J64" s="4">
         <v>-5.5999999999999999E-3</v>
       </c>
-      <c r="K64" s="6">
+      <c r="K64" s="5">
         <v>-5.2808988764045051E-2</v>
       </c>
-      <c r="L64" s="6">
+      <c r="L64" s="5">
         <v>-2.1910112359550538E-2</v>
       </c>
       <c r="M64" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" s="3" customFormat="1">
       <c r="A65" s="2">
         <v>42725</v>
       </c>
@@ -3957,17 +3959,17 @@
       <c r="J65" s="4">
         <v>0.1268</v>
       </c>
-      <c r="K65" s="6">
+      <c r="K65" s="5">
         <v>8.2118561710398552E-2</v>
       </c>
-      <c r="L65" s="6">
+      <c r="L65" s="5">
         <v>7.0942662779397425E-2</v>
       </c>
       <c r="M65" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" s="3" customFormat="1">
       <c r="A66" s="2">
         <v>42816</v>
       </c>
@@ -3998,17 +4000,17 @@
       <c r="J66" s="4">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="K66" s="6">
+      <c r="K66" s="5">
         <v>9.4446543256516913E-2</v>
       </c>
-      <c r="L66" s="6">
+      <c r="L66" s="5">
         <v>8.122402720060462E-2</v>
       </c>
       <c r="M66" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" s="3" customFormat="1">
       <c r="A67" s="2">
         <v>42116</v>
       </c>
@@ -4039,17 +4041,17 @@
       <c r="J67" s="4">
         <v>0.1045</v>
       </c>
-      <c r="K67" s="6">
+      <c r="K67" s="5">
         <v>0.12228887863405613</v>
       </c>
-      <c r="L67" s="6">
+      <c r="L67" s="5">
         <v>7.7526534379326328E-2</v>
       </c>
       <c r="M67" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:13" s="3" customFormat="1">
       <c r="A68" s="2">
         <v>42200</v>
       </c>
@@ -4080,17 +4082,17 @@
       <c r="J68" s="4">
         <v>-3.6799999999999999E-2</v>
       </c>
-      <c r="K68" s="6">
+      <c r="K68" s="5">
         <v>-4.1032148900169152E-2</v>
       </c>
-      <c r="L68" s="6">
+      <c r="L68" s="5">
         <v>5.4991539763113995E-3</v>
       </c>
       <c r="M68" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:13" s="3" customFormat="1">
       <c r="A69" s="2">
         <v>42298</v>
       </c>
@@ -4121,17 +4123,17 @@
       <c r="J69" s="4">
         <v>0.1008</v>
       </c>
-      <c r="K69" s="6">
+      <c r="K69" s="5">
         <v>0.11097230897355814</v>
       </c>
-      <c r="L69" s="6">
+      <c r="L69" s="5">
         <v>0.13220903601915479</v>
       </c>
       <c r="M69" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13" s="3" customFormat="1">
       <c r="A70" s="2">
         <v>42396</v>
       </c>
@@ -4162,17 +4164,17 @@
       <c r="J70" s="4">
         <v>5.8299999999999998E-2</v>
       </c>
-      <c r="K70" s="6">
+      <c r="K70" s="5">
         <v>-1.1525163273147232E-3</v>
       </c>
-      <c r="L70" s="6">
+      <c r="L70" s="5">
         <v>-4.5524394928928236E-2</v>
       </c>
       <c r="M70" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13" s="3" customFormat="1">
       <c r="A71" s="2">
         <v>42480</v>
       </c>
@@ -4203,17 +4205,17 @@
       <c r="J71" s="4">
         <v>-7.17E-2</v>
       </c>
-      <c r="K71" s="6">
+      <c r="K71" s="5">
         <v>-0.10541412692721408</v>
       </c>
-      <c r="L71" s="6">
+      <c r="L71" s="5">
         <v>-0.10469702402294734</v>
       </c>
       <c r="M71" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13" s="3" customFormat="1">
       <c r="A72" s="2">
         <v>42564</v>
       </c>
@@ -4244,17 +4246,17 @@
       <c r="J72" s="4">
         <v>5.3100000000000001E-2</v>
       </c>
-      <c r="K72" s="6">
+      <c r="K72" s="5">
         <v>6.9127896025616753E-2</v>
       </c>
-      <c r="L72" s="6">
+      <c r="L72" s="5">
         <v>6.5737427010736482E-2</v>
       </c>
       <c r="M72" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:13" s="3" customFormat="1">
       <c r="A73" s="2">
         <v>42662</v>
       </c>
@@ -4285,17 +4287,17 @@
       <c r="J73" s="4">
         <v>4.2099999999999999E-2</v>
       </c>
-      <c r="K73" s="6">
+      <c r="K73" s="5">
         <v>4.9781659388646204E-2</v>
       </c>
-      <c r="L73" s="6">
+      <c r="L73" s="5">
         <v>3.4235807860262035E-2</v>
       </c>
       <c r="M73" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13" s="3" customFormat="1">
       <c r="A74" s="2">
         <v>42760</v>
       </c>
@@ -4326,17 +4328,17 @@
       <c r="J74" s="4">
         <v>2.35E-2</v>
       </c>
-      <c r="K74" s="6">
+      <c r="K74" s="5">
         <v>-1.7115294849852081E-2</v>
       </c>
-      <c r="L74" s="6">
+      <c r="L74" s="5">
         <v>-3.2674653804262155E-3</v>
       </c>
       <c r="M74" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13" s="3" customFormat="1">
       <c r="A75" s="2">
         <v>42109</v>
       </c>
@@ -4367,17 +4369,17 @@
       <c r="J75" s="4">
         <v>0.18210000000000001</v>
       </c>
-      <c r="K75" s="6">
+      <c r="K75" s="5">
         <v>0.17299764428739683</v>
       </c>
-      <c r="L75" s="6">
+      <c r="L75" s="5">
         <v>0.18389281507656063</v>
       </c>
       <c r="M75" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13" s="3" customFormat="1">
       <c r="A76" s="2">
         <v>42200</v>
       </c>
@@ -4408,17 +4410,17 @@
       <c r="J76" s="4">
         <v>0.1802</v>
       </c>
-      <c r="K76" s="6">
+      <c r="K76" s="5">
         <v>0.13624783450524824</v>
       </c>
-      <c r="L76" s="6">
+      <c r="L76" s="5">
         <v>9.1205543666564859E-2</v>
       </c>
       <c r="M76" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:13" s="3" customFormat="1">
       <c r="A77" s="2">
         <v>42291</v>
       </c>
@@ -4449,17 +4451,17 @@
       <c r="J77" s="4">
         <v>-8.2900000000000001E-2</v>
       </c>
-      <c r="K77" s="6">
+      <c r="K77" s="5">
         <v>-0.11131270978862384</v>
       </c>
-      <c r="L77" s="6">
+      <c r="L77" s="5">
         <v>-4.0188696362151943E-2</v>
       </c>
       <c r="M77" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:13" s="3" customFormat="1">
       <c r="A78" s="2">
         <v>42382</v>
       </c>
@@ -4490,17 +4492,17 @@
       <c r="J78" s="4">
         <v>-1.4E-3</v>
       </c>
-      <c r="K78" s="6">
+      <c r="K78" s="5">
         <v>-9.3243117990545965E-2</v>
       </c>
-      <c r="L78" s="6">
+      <c r="L78" s="5">
         <v>-0.1520066734637131</v>
       </c>
       <c r="M78" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:13" s="3" customFormat="1">
       <c r="A79" s="2">
         <v>42473</v>
       </c>
@@ -4531,17 +4533,17 @@
       <c r="J79" s="4">
         <v>-0.12970000000000001</v>
       </c>
-      <c r="K79" s="6">
+      <c r="K79" s="5">
         <v>-0.13690036900369007</v>
       </c>
-      <c r="L79" s="6">
+      <c r="L79" s="5">
         <v>-0.14105166051660523</v>
       </c>
       <c r="M79" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="80" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:13" s="3" customFormat="1">
       <c r="A80" s="2">
         <v>42564</v>
       </c>
@@ -4572,17 +4574,17 @@
       <c r="J80" s="4">
         <v>-0.1313</v>
       </c>
-      <c r="K80" s="6">
+      <c r="K80" s="5">
         <v>-0.1128428296731101</v>
       </c>
-      <c r="L80" s="6">
+      <c r="L80" s="5">
         <v>-4.4934723206153215E-2</v>
       </c>
       <c r="M80" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:13" s="3" customFormat="1">
       <c r="A81" s="2">
         <v>42655</v>
       </c>
@@ -4613,17 +4615,17 @@
       <c r="J81" s="4">
         <v>0.1903</v>
       </c>
-      <c r="K81" s="6">
+      <c r="K81" s="5">
         <v>0.27585170340681375</v>
       </c>
-      <c r="L81" s="6">
+      <c r="L81" s="5">
         <v>0.25120240480961931</v>
       </c>
       <c r="M81" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:13" s="3" customFormat="1">
       <c r="A82" s="2">
         <v>42753</v>
       </c>
@@ -4654,17 +4656,17 @@
       <c r="J82" s="4">
         <v>3.8600000000000002E-2</v>
       </c>
-      <c r="K82" s="6">
+      <c r="K82" s="5">
         <v>4.6975836710190677E-2</v>
       </c>
-      <c r="L82" s="6">
+      <c r="L82" s="5">
         <v>5.6431037070388879E-2</v>
       </c>
       <c r="M82" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:13" s="3" customFormat="1">
       <c r="A83" s="2">
         <v>42130</v>
       </c>
@@ -4695,17 +4697,17 @@
       <c r="J83" s="4">
         <v>-7.3999999999999996E-2</v>
       </c>
-      <c r="K83" s="6">
+      <c r="K83" s="5">
         <v>-5.3357047576700678E-2</v>
       </c>
-      <c r="L83" s="6">
+      <c r="L83" s="5">
         <v>-7.1142730102267571E-2</v>
       </c>
       <c r="M83" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:13" s="3" customFormat="1">
       <c r="A84" s="2">
         <v>42221</v>
       </c>
@@ -4736,17 +4738,17 @@
       <c r="J84" s="4">
         <v>0.1237</v>
       </c>
-      <c r="K84" s="6">
+      <c r="K84" s="5">
         <v>0.15012224938875307</v>
       </c>
-      <c r="L84" s="6">
+      <c r="L84" s="5">
         <v>8.3618581907090483E-2</v>
       </c>
       <c r="M84" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:13" s="3" customFormat="1">
       <c r="A85" s="2">
         <v>42307</v>
       </c>
@@ -4777,17 +4779,17 @@
       <c r="J85" s="4">
         <v>0.1386</v>
       </c>
-      <c r="K85" s="6">
+      <c r="K85" s="5">
         <v>9.7076867556838531E-2</v>
       </c>
-      <c r="L85" s="6">
+      <c r="L85" s="5">
         <v>0.12306026705160589</v>
       </c>
       <c r="M85" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:13" s="3" customFormat="1">
       <c r="A86" s="2">
         <v>42412</v>
       </c>
@@ -4818,17 +4820,17 @@
       <c r="J86" s="4">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="K86" s="6">
+      <c r="K86" s="5">
         <v>0.15039768618944316</v>
       </c>
-      <c r="L86" s="6">
+      <c r="L86" s="5">
         <v>0.19088937093275482</v>
       </c>
       <c r="M86" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:13" s="3" customFormat="1">
       <c r="A87" s="2">
         <v>42496</v>
       </c>
@@ -4859,17 +4861,17 @@
       <c r="J87" s="4">
         <v>0.15210000000000001</v>
       </c>
-      <c r="K87" s="6">
+      <c r="K87" s="5">
         <v>0.22434635929153779</v>
       </c>
-      <c r="L87" s="6">
+      <c r="L87" s="5">
         <v>0.28338487489457398</v>
       </c>
       <c r="M87" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:13" s="3" customFormat="1">
       <c r="A88" s="2">
         <v>42587</v>
       </c>
@@ -4900,17 +4902,17 @@
       <c r="J88" s="4">
         <v>5.5899999999999998E-2</v>
       </c>
-      <c r="K88" s="6">
+      <c r="K88" s="5">
         <v>4.020100502512558E-2</v>
       </c>
-      <c r="L88" s="6">
+      <c r="L88" s="5">
         <v>3.0653266331658324E-2</v>
       </c>
       <c r="M88" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:13" s="3" customFormat="1">
       <c r="A89" s="2">
         <v>42678</v>
       </c>
@@ -4941,17 +4943,17 @@
       <c r="J89" s="4">
         <v>0.29809999999999998</v>
       </c>
-      <c r="K89" s="6">
+      <c r="K89" s="5">
         <v>0.36328759037922387</v>
       </c>
-      <c r="L89" s="6">
+      <c r="L89" s="5">
         <v>0.38940534159657658</v>
       </c>
       <c r="M89" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:13" s="3" customFormat="1">
       <c r="A90" s="2">
         <v>42769</v>
       </c>
@@ -4982,17 +4984,17 @@
       <c r="J90" s="4">
         <v>-2.3699999999999999E-2</v>
       </c>
-      <c r="K90" s="6">
+      <c r="K90" s="5">
         <v>-7.844990548204156E-2</v>
       </c>
-      <c r="L90" s="6">
+      <c r="L90" s="5">
         <v>-0.12820072177350061</v>
       </c>
       <c r="M90" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:13" s="3" customFormat="1">
       <c r="A91" s="2">
         <v>42116</v>
       </c>
@@ -5023,17 +5025,17 @@
       <c r="J91" s="4">
         <v>-0.18179999999999999</v>
       </c>
-      <c r="K91" s="6">
+      <c r="K91" s="5">
         <v>-0.26674409601238858</v>
       </c>
-      <c r="L91" s="6">
+      <c r="L91" s="5">
         <v>-0.27777777777777768</v>
       </c>
       <c r="M91" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="92" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:13" s="3" customFormat="1">
       <c r="A92" s="2">
         <v>42207</v>
       </c>
@@ -5064,17 +5066,17 @@
       <c r="J92" s="4">
         <v>-0.14499999999999999</v>
       </c>
-      <c r="K92" s="6">
+      <c r="K92" s="5">
         <v>-0.19704433497536944</v>
       </c>
-      <c r="L92" s="6">
+      <c r="L92" s="5">
         <v>-0.18938149972632723</v>
       </c>
       <c r="M92" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:13" s="3" customFormat="1">
       <c r="A93" s="2">
         <v>42298</v>
       </c>
@@ -5105,17 +5107,17 @@
       <c r="J93" s="4">
         <v>-1.4999999999999999E-2</v>
       </c>
-      <c r="K93" s="6">
+      <c r="K93" s="5">
         <v>-7.0516911295469109E-2</v>
       </c>
-      <c r="L93" s="6">
+      <c r="L93" s="5">
         <v>-0.13688576898532223</v>
       </c>
       <c r="M93" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="94" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:13" s="3" customFormat="1">
       <c r="A94" s="2">
         <v>42410</v>
       </c>
@@ -5146,17 +5148,17 @@
       <c r="J94" s="4">
         <v>-4.4699999999999997E-2</v>
       </c>
-      <c r="K94" s="6">
+      <c r="K94" s="5">
         <v>0.2303070761014685</v>
       </c>
-      <c r="L94" s="6">
+      <c r="L94" s="5">
         <v>0.17423230974632831</v>
       </c>
       <c r="M94" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="95" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:13" s="3" customFormat="1">
       <c r="A95" s="2">
         <v>42480</v>
       </c>
@@ -5187,17 +5189,17 @@
       <c r="J95" s="4">
         <v>-0.1628</v>
       </c>
-      <c r="K95" s="6">
+      <c r="K95" s="5">
         <v>-0.21070422535211264</v>
       </c>
-      <c r="L95" s="6">
+      <c r="L95" s="5">
         <v>-0.17577464788732389</v>
       </c>
       <c r="M95" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="96" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:13" s="3" customFormat="1">
       <c r="A96" s="2">
         <v>42571</v>
       </c>
@@ -5228,17 +5230,17 @@
       <c r="J96" s="4">
         <v>-0.14530000000000001</v>
       </c>
-      <c r="K96" s="6">
+      <c r="K96" s="5">
         <v>-0.1100271002710026</v>
       </c>
-      <c r="L96" s="6">
+      <c r="L96" s="5">
         <v>1.2466124661246747E-2</v>
       </c>
       <c r="M96" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="97" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:13" s="3" customFormat="1">
       <c r="A97" s="2">
         <v>42669</v>
       </c>
@@ -5269,17 +5271,17 @@
       <c r="J97" s="4">
         <v>6.4000000000000003E-3</v>
       </c>
-      <c r="K97" s="6">
+      <c r="K97" s="5">
         <v>1.8507807981492208E-2</v>
       </c>
-      <c r="L97" s="6">
+      <c r="L97" s="5">
         <v>0.10641989589358003</v>
       </c>
       <c r="M97" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="98" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:13" s="3" customFormat="1">
       <c r="A98" s="2">
         <v>42774</v>
       </c>
@@ -5310,58 +5312,58 @@
       <c r="J98" s="4">
         <v>-0.1234</v>
       </c>
-      <c r="K98" s="6">
+      <c r="K98" s="5">
         <v>-0.10576923076923084</v>
       </c>
-      <c r="L98" s="6">
+      <c r="L98" s="5">
         <v>-0.14369658119658113</v>
       </c>
       <c r="M98" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="8">
+    <row r="99" spans="1:13" s="6" customFormat="1">
+      <c r="A99" s="7">
         <v>42059</v>
       </c>
-      <c r="B99" s="7">
+      <c r="B99" s="6">
         <v>0.26258889770312399</v>
       </c>
-      <c r="C99" s="7">
+      <c r="C99" s="6">
         <v>0.26258889770312399</v>
       </c>
-      <c r="D99" s="7">
+      <c r="D99" s="6">
         <v>0.26258889770312399</v>
       </c>
-      <c r="E99" s="7">
+      <c r="E99" s="6">
         <v>0.26258889770312399</v>
       </c>
-      <c r="F99" s="7">
+      <c r="F99" s="6">
         <v>-8.9457002296876031E-2</v>
       </c>
-      <c r="G99" s="7">
+      <c r="G99" s="6">
         <v>-8.9457002296876031E-2</v>
       </c>
-      <c r="H99" s="7">
+      <c r="H99" s="6">
         <v>-8.9457002296876031E-2</v>
       </c>
-      <c r="I99" s="7">
+      <c r="I99" s="6">
         <v>-8.9457002296876031E-2</v>
       </c>
-      <c r="J99" s="6">
+      <c r="J99" s="5">
         <v>-9.9199999999999997E-2</v>
       </c>
-      <c r="K99" s="6">
+      <c r="K99" s="5">
         <v>-0.1018</v>
       </c>
-      <c r="L99" s="6">
+      <c r="L99" s="5">
         <v>-0.1512</v>
       </c>
-      <c r="M99" s="7" t="s">
+      <c r="M99" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:13">
       <c r="A100" s="1">
         <v>42145</v>
       </c>
@@ -5389,20 +5391,20 @@
       <c r="I100">
         <v>-0.49299305878829591</v>
       </c>
-      <c r="J100" s="6">
+      <c r="J100" s="5">
         <v>2.75E-2</v>
       </c>
-      <c r="K100" s="6">
+      <c r="K100" s="5">
         <v>-1.2699999999999999E-2</v>
       </c>
-      <c r="L100" s="6">
+      <c r="L100" s="5">
         <v>-2.69E-2</v>
       </c>
-      <c r="M100" s="7" t="s">
+      <c r="M100" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:13">
       <c r="A101" s="1">
         <v>42236</v>
       </c>
@@ -5430,20 +5432,20 @@
       <c r="I101">
         <v>5.5964987184644432E-2</v>
       </c>
-      <c r="J101" s="6">
+      <c r="J101" s="5">
         <v>4.4000000000000003E-3</v>
       </c>
-      <c r="K101" s="6">
+      <c r="K101" s="5">
         <v>1.61E-2</v>
       </c>
-      <c r="L101" s="6">
+      <c r="L101" s="5">
         <v>2.8500000000000001E-2</v>
       </c>
-      <c r="M101" s="7" t="s">
+      <c r="M101" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:13">
       <c r="A102" s="1">
         <v>42332</v>
       </c>
@@ -5471,20 +5473,20 @@
       <c r="I102">
         <v>0.22981548475597935</v>
       </c>
-      <c r="J102" s="6">
+      <c r="J102" s="5">
         <v>-0.1366</v>
       </c>
-      <c r="K102" s="6">
+      <c r="K102" s="5">
         <v>-0.1837</v>
       </c>
-      <c r="L102" s="6">
+      <c r="L102" s="5">
         <v>-0.17280000000000001</v>
       </c>
-      <c r="M102" s="7" t="s">
+      <c r="M102" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:13">
       <c r="A103" s="1">
         <v>42424</v>
       </c>
@@ -5512,20 +5514,20 @@
       <c r="I103">
         <v>1.2102463568039723</v>
       </c>
-      <c r="J103" s="6">
+      <c r="J103" s="5">
         <v>-4.4400000000000002E-2</v>
       </c>
-      <c r="K103" s="6">
+      <c r="K103" s="5">
         <v>7.4000000000000003E-3</v>
       </c>
-      <c r="L103" s="6">
+      <c r="L103" s="5">
         <v>4.99E-2</v>
       </c>
-      <c r="M103" s="7" t="s">
+      <c r="M103" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:13">
       <c r="A104" s="1">
         <v>42515</v>
       </c>
@@ -5553,20 +5555,20 @@
       <c r="I104">
         <v>1.2441977551362875</v>
       </c>
-      <c r="J104" s="6">
+      <c r="J104" s="5">
         <v>6.8900000000000003E-2</v>
       </c>
-      <c r="K104" s="6">
+      <c r="K104" s="5">
         <v>0.10979999999999999</v>
       </c>
-      <c r="L104" s="6">
+      <c r="L104" s="5">
         <v>0.13439999999999999</v>
       </c>
-      <c r="M104" s="7" t="s">
+      <c r="M104" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:13">
       <c r="A105" s="1">
         <v>42606</v>
       </c>
@@ -5594,20 +5596,20 @@
       <c r="I105">
         <v>0.23628943175182515</v>
       </c>
-      <c r="J105" s="6">
+      <c r="J105" s="5">
         <v>-2.0999999999999999E-3</v>
       </c>
-      <c r="K105" s="6">
+      <c r="K105" s="5">
         <v>-2.0999999999999999E-3</v>
       </c>
-      <c r="L105" s="6">
+      <c r="L105" s="5">
         <v>1.6E-2</v>
       </c>
-      <c r="M105" s="7" t="s">
+      <c r="M105" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:13">
       <c r="A106" s="1">
         <v>42696</v>
       </c>
@@ -5635,20 +5637,20 @@
       <c r="I106">
         <v>0.15482076673022449</v>
       </c>
-      <c r="J106" s="6">
+      <c r="J106" s="5">
         <v>-6.7699999999999996E-2</v>
       </c>
-      <c r="K106" s="6">
+      <c r="K106" s="5">
         <v>-3.4500000000000003E-2</v>
       </c>
-      <c r="L106" s="6">
+      <c r="L106" s="5">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="M106" s="7" t="s">
+      <c r="M106" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:13">
       <c r="A107" s="1">
         <v>42788</v>
       </c>
@@ -5676,16 +5678,16 @@
       <c r="I107">
         <v>0.57527262656942268</v>
       </c>
-      <c r="J107" s="6">
-        <v>-6.7699999999999996E-2</v>
-      </c>
-      <c r="K107" s="6">
-        <v>-3.4500000000000003E-2</v>
-      </c>
-      <c r="L107" s="6">
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="M107" s="7" t="s">
+      <c r="J107" s="5">
+        <v>8.6419753086419915E-2</v>
+      </c>
+      <c r="K107" s="5">
+        <v>8.7654320987654355E-2</v>
+      </c>
+      <c r="L107" s="5">
+        <v>6.9135802469135976E-2</v>
+      </c>
+      <c r="M107" s="6" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
consolidating all categorized averages
</commit_message>
<xml_diff>
--- a/data/general/all_averages.xlsx
+++ b/data/general/all_averages.xlsx
@@ -22,15 +22,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="34">
   <si>
     <t>Company</t>
   </si>
@@ -109,12 +106,36 @@
   <si>
     <t>PxCh 10 Trading Days Later</t>
   </si>
+  <si>
+    <t>ENV 1 week average sentiment</t>
+  </si>
+  <si>
+    <t>ECON 1 week average sentiment</t>
+  </si>
+  <si>
+    <t>LEAD 1 week average sentiment</t>
+  </si>
+  <si>
+    <t>LEGAL 1 week average sentiment</t>
+  </si>
+  <si>
+    <t>SOC 1 week average sentiment</t>
+  </si>
+  <si>
+    <t>SOURCE 1 week average sentiment</t>
+  </si>
+  <si>
+    <t>PxCh 5-1 Trading Days Later</t>
+  </si>
+  <si>
+    <t>PxCh 10-1 Trading Days Later</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,6 +166,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -383,7 +411,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -393,6 +421,14 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="218">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -947,7 +983,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -999,7 +1035,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1201,10 +1237,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M107"/>
+  <dimension ref="A1:U107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F95" workbookViewId="0">
-      <selection activeCell="I102" sqref="I102"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="I94" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="M107" sqref="M107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1220,9 +1259,11 @@
     <col min="10" max="10" width="8.453125" customWidth="1"/>
     <col min="11" max="11" width="20.453125" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.453125" style="5" customWidth="1"/>
+    <col min="13" max="14" width="20.453125" style="13" customWidth="1"/>
+    <col min="18" max="18" width="8.81640625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1259,11 +1300,35 @@
       <c r="L1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="S1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T1" t="s">
+        <v>30</v>
+      </c>
+      <c r="U1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <f>[1]apple_averages!A12</f>
         <v>42123</v>
@@ -1310,11 +1375,35 @@
       <c r="L2" s="5">
         <v>-4.7719562759140688E-2</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="15">
+        <v>-1.4246323529411908E-2</v>
+      </c>
+      <c r="N2" s="15">
+        <v>-3.2475490196078538E-2</v>
+      </c>
+      <c r="O2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P2" s="10">
+        <v>0.23765616054022901</v>
+      </c>
+      <c r="Q2">
+        <v>-0.35349033009090902</v>
+      </c>
+      <c r="R2" s="12">
+        <v>-0.243802899307692</v>
+      </c>
+      <c r="S2">
+        <v>-1.2260515431363599</v>
+      </c>
+      <c r="T2">
+        <v>-3.0825328490000001</v>
+      </c>
+      <c r="U2">
+        <v>-0.704774495061538</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <f>[1]apple_averages!A24</f>
         <v>42207</v>
@@ -1361,11 +1450,35 @@
       <c r="L3" s="5">
         <v>-0.12321223709369022</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="15">
+        <v>-1.4694138316562855E-2</v>
+      </c>
+      <c r="N3" s="15">
+        <v>-8.4491295320236359E-2</v>
+      </c>
+      <c r="O3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P3" s="10">
+        <v>1.30657265856163E-2</v>
+      </c>
+      <c r="Q3">
+        <v>-0.73002238513333295</v>
+      </c>
+      <c r="R3" s="12">
+        <v>0.39191692783673399</v>
+      </c>
+      <c r="S3">
+        <v>-0.94239202553846102</v>
+      </c>
+      <c r="T3">
+        <v>-2.3191094620000001</v>
+      </c>
+      <c r="U3">
+        <v>-0.201582874181818</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <f>[1]apple_averages!A38</f>
         <v>42305</v>
@@ -1412,11 +1525,35 @@
       <c r="L4" s="5">
         <v>1.9380183326058509E-2</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="15">
+        <v>2.7668315586484526E-2</v>
+      </c>
+      <c r="N4" s="15">
+        <v>-2.0960845141276052E-2</v>
+      </c>
+      <c r="O4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P4" s="10">
+        <v>0.55132851654418602</v>
+      </c>
+      <c r="Q4">
+        <v>0.55927167056666605</v>
+      </c>
+      <c r="R4" s="12">
+        <v>3.8828469735294101E-2</v>
+      </c>
+      <c r="S4">
+        <v>-0.831827903588235</v>
+      </c>
+      <c r="T4">
+        <v>2.3513446139999998</v>
+      </c>
+      <c r="U4">
+        <v>0.65306930802564001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <f>[1]apple_averages!A51</f>
         <v>42396</v>
@@ -1463,11 +1600,35 @@
       <c r="L5" s="4">
         <v>-5.0005000500049968E-2</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="16">
+        <v>1.1299999999999999E-2</v>
+      </c>
+      <c r="N5" s="14">
+        <v>1.6805823164204536E-2</v>
+      </c>
+      <c r="O5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P5" s="10">
+        <v>7.4981258443137494E-2</v>
+      </c>
+      <c r="Q5">
+        <v>-0.90693851342105203</v>
+      </c>
+      <c r="R5" s="12">
+        <v>-0.765250293522727</v>
+      </c>
+      <c r="S5">
+        <v>0.32018858273214201</v>
+      </c>
+      <c r="T5">
+        <v>-1.6603642270000001</v>
+      </c>
+      <c r="U5">
+        <v>-0.28163474560714202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <f>[1]apple_averages!A64</f>
         <v>42487</v>
@@ -1514,11 +1675,35 @@
       <c r="L6" s="4">
         <v>-0.1047436511739338</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="14">
+        <v>-2.6988345941525101E-2</v>
+      </c>
+      <c r="N6" s="14">
+        <v>-4.4980576569208619E-2</v>
+      </c>
+      <c r="O6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P6" s="10">
+        <v>-1.4279912061798501</v>
+      </c>
+      <c r="Q6">
+        <v>-2.8369935139833302</v>
+      </c>
+      <c r="R6" s="12">
+        <v>-0.76492461746739104</v>
+      </c>
+      <c r="S6">
+        <v>-1.8402937980973999</v>
+      </c>
+      <c r="T6">
+        <v>-2.4921069230000001</v>
+      </c>
+      <c r="U6">
+        <v>-1.3742978682739699</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <f>[1]apple_averages!A77</f>
         <v>42578</v>
@@ -1565,11 +1750,35 @@
       <c r="L7" s="4">
         <v>0.1255818764870178</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="14">
+        <v>1.4861583292860692E-2</v>
+      </c>
+      <c r="N7" s="14">
+        <v>5.6920835356969457E-2</v>
+      </c>
+      <c r="O7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P7" s="10">
+        <v>0.40719659536097502</v>
+      </c>
+      <c r="Q7">
+        <v>0.16622261208695599</v>
+      </c>
+      <c r="R7" s="12">
+        <v>0.96697224184374997</v>
+      </c>
+      <c r="S7">
+        <v>-1.2731506452289101</v>
+      </c>
+      <c r="T7">
+        <v>-0.63948840900000004</v>
+      </c>
+      <c r="U7">
+        <v>0.212377084212962</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <f>[1]apple_averages!A90</f>
         <v>42669</v>
@@ -1616,11 +1825,35 @@
       <c r="L8" s="4">
         <v>-6.0803382663847771E-2</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="14">
+        <v>-3.5470196383770247E-2</v>
+      </c>
+      <c r="N8" s="14">
+        <v>-4.749529527735441E-3</v>
+      </c>
+      <c r="O8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P8" s="10">
+        <v>0.31244922687499999</v>
+      </c>
+      <c r="Q8">
+        <v>-0.99884359282222202</v>
+      </c>
+      <c r="R8" s="12">
+        <v>-0.22696448967567501</v>
+      </c>
+      <c r="S8">
+        <v>-2.0867438297073102</v>
+      </c>
+      <c r="T8">
+        <v>-1.74354736</v>
+      </c>
+      <c r="U8">
+        <v>-0.210142228886363</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <f>[1]apple_averages!A104</f>
         <v>42767</v>
@@ -1667,11 +1900,35 @@
       <c r="L9" s="4">
         <v>0.11264936135146275</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="14">
+        <v>2.1592233009708695E-2</v>
+      </c>
+      <c r="N9" s="14">
+        <v>4.8699029126213711E-2</v>
+      </c>
+      <c r="O9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P9" s="10">
+        <v>0.77164202624725298</v>
+      </c>
+      <c r="Q9">
+        <v>0.21543620917241299</v>
+      </c>
+      <c r="R9" s="12">
+        <v>-0.285707523632653</v>
+      </c>
+      <c r="S9">
+        <v>-1.83001872276829</v>
+      </c>
+      <c r="T9">
+        <v>-1.184791143</v>
+      </c>
+      <c r="U9">
+        <v>0.34735664183333298</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>42116</v>
       </c>
@@ -1708,11 +1965,35 @@
       <c r="L10" s="4">
         <v>9.4592169029975137E-2</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="M10" s="14">
+        <v>-5.2392720736913145E-2</v>
+      </c>
+      <c r="N10" s="14">
+        <v>-4.0934621433385776E-2</v>
+      </c>
+      <c r="O10" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P10" s="11">
+        <v>0.66819772496341401</v>
+      </c>
+      <c r="Q10">
+        <v>1.5994626257187501</v>
+      </c>
+      <c r="R10" s="12">
+        <v>0.67639085776595698</v>
+      </c>
+      <c r="S10">
+        <v>-0.120399037</v>
+      </c>
+      <c r="T10">
+        <v>-0.88180270000000005</v>
+      </c>
+      <c r="U10">
+        <v>0.95220103807547096</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>42207</v>
       </c>
@@ -1749,11 +2030,35 @@
       <c r="L11" s="4">
         <v>9.805466838110255E-2</v>
       </c>
-      <c r="M11" s="3" t="s">
+      <c r="M11" s="14">
+        <v>1.3864228778663445E-2</v>
+      </c>
+      <c r="N11" s="14">
+        <v>7.5554380265296928E-5</v>
+      </c>
+      <c r="O11" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P11" s="10">
+        <v>1.73456948470379</v>
+      </c>
+      <c r="Q11">
+        <v>1.9222736722857099</v>
+      </c>
+      <c r="R11" s="12">
+        <v>1.0313159572333299</v>
+      </c>
+      <c r="S11">
+        <v>1.1432238777777699</v>
+      </c>
+      <c r="T11">
+        <v>0.484848485</v>
+      </c>
+      <c r="U11">
+        <v>1.29090140207142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>42298</v>
       </c>
@@ -1790,11 +2095,35 @@
       <c r="L12" s="4">
         <v>0.16268553492578608</v>
       </c>
-      <c r="M12" s="3" t="s">
+      <c r="M12" s="14">
+        <v>4.5940937849523467E-2</v>
+      </c>
+      <c r="N12" s="14">
+        <v>9.4519473148256372E-2</v>
+      </c>
+      <c r="O12" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P12" s="10">
+        <v>1.99091683159375</v>
+      </c>
+      <c r="Q12">
+        <v>1.6424648980000001</v>
+      </c>
+      <c r="R12" s="12">
+        <v>2.8843341347999898</v>
+      </c>
+      <c r="S12">
+        <v>-1.0291595200000001</v>
+      </c>
+      <c r="T12">
+        <v>-1.363326517</v>
+      </c>
+      <c r="U12">
+        <v>1.38899286228571</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>42396</v>
       </c>
@@ -1831,11 +2160,35 @@
       <c r="L13" s="4">
         <v>-0.20701975289210672</v>
       </c>
-      <c r="M13" s="3" t="s">
+      <c r="M13" s="14">
+        <v>-8.6439522998296492E-2</v>
+      </c>
+      <c r="N13" s="14">
+        <v>-0.14170357751277685</v>
+      </c>
+      <c r="O13" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P13" s="10">
+        <v>1.61596470728571</v>
+      </c>
+      <c r="Q13">
+        <v>1.2590412284482699</v>
+      </c>
+      <c r="R13" s="12">
+        <v>1.5001542141818101</v>
+      </c>
+      <c r="S13">
+        <v>0.75032181961904698</v>
+      </c>
+      <c r="T13">
+        <v>-3.5897435899999999</v>
+      </c>
+      <c r="U13">
+        <v>0.57676031939999906</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>42487</v>
       </c>
@@ -1872,11 +2225,35 @@
       <c r="L14" s="4">
         <v>0.19257475083056463</v>
       </c>
-      <c r="M14" s="3" t="s">
+      <c r="M14" s="14">
+        <v>-7.5804666535272958E-4</v>
+      </c>
+      <c r="N14" s="14">
+        <v>8.8448884913355119E-2</v>
+      </c>
+      <c r="O14" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P14" s="10">
+        <v>0.75320143634782599</v>
+      </c>
+      <c r="Q14">
+        <v>1.830663616</v>
+      </c>
+      <c r="R14" s="12">
+        <v>0.17421833754054</v>
+      </c>
+      <c r="S14">
+        <v>-1.86980872576923</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>1.13357106870833</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>42578</v>
       </c>
@@ -1913,11 +2290,35 @@
       <c r="L15" s="4">
         <v>2.4753856579104783E-2</v>
       </c>
-      <c r="M15" s="3" t="s">
+      <c r="M15" s="14">
+        <v>2.5829917897761678E-3</v>
+      </c>
+      <c r="N15" s="14">
+        <v>1.6380912217814902E-2</v>
+      </c>
+      <c r="O15" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P15" s="10">
+        <v>1.68456187886956</v>
+      </c>
+      <c r="Q15">
+        <v>1.48857681199999</v>
+      </c>
+      <c r="R15" s="12">
+        <v>1.71675497138596</v>
+      </c>
+      <c r="S15">
+        <v>1.655981001</v>
+      </c>
+      <c r="T15">
+        <v>-1.7948717949999999</v>
+      </c>
+      <c r="U15">
+        <v>0.62498885876923005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>42669</v>
       </c>
@@ -1954,11 +2355,35 @@
       <c r="L16" s="4">
         <v>-9.2844225035436767E-2</v>
       </c>
-      <c r="M16" s="3" t="s">
+      <c r="M16" s="14">
+        <v>-1.1966714756801444E-2</v>
+      </c>
+      <c r="N16" s="14">
+        <v>-4.3719084913437789E-2</v>
+      </c>
+      <c r="O16" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P16" s="10">
+        <v>1.8227574998629399</v>
+      </c>
+      <c r="Q16">
+        <v>1.71222300237837</v>
+      </c>
+      <c r="R16" s="12">
+        <v>-2.0196541138490498</v>
+      </c>
+      <c r="S16">
+        <v>-0.60013580849999903</v>
+      </c>
+      <c r="T16">
+        <v>1.533546326</v>
+      </c>
+      <c r="U16">
+        <v>-1.3488911984285701</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>42767</v>
       </c>
@@ -1995,11 +2420,35 @@
       <c r="L17" s="4">
         <v>4.9883921662003949E-3</v>
       </c>
-      <c r="M17" s="3" t="s">
+      <c r="M17" s="14">
+        <v>1.3774376697111679E-2</v>
+      </c>
+      <c r="N17" s="14">
+        <v>4.1890891137990494E-2</v>
+      </c>
+      <c r="O17" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P17" s="10">
+        <v>2.0374137991499999</v>
+      </c>
+      <c r="Q17">
+        <v>0.89814616123076896</v>
+      </c>
+      <c r="R17" s="12">
+        <v>0.96746602973684104</v>
+      </c>
+      <c r="S17">
+        <v>0.83633914539999898</v>
+      </c>
+      <c r="T17">
+        <v>-2.5142166619999999</v>
+      </c>
+      <c r="U17">
+        <v>1.2049149928571401E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>42109</v>
       </c>
@@ -2036,11 +2485,35 @@
       <c r="L18" s="4">
         <v>-0.21254355400696878</v>
       </c>
-      <c r="M18" s="3" t="s">
+      <c r="M18" s="14">
+        <v>-9.68992248062015E-2</v>
+      </c>
+      <c r="N18" s="14">
+        <v>-0.12403100775193809</v>
+      </c>
+      <c r="O18" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P18" s="10">
+        <v>0.19965354599999999</v>
+      </c>
+      <c r="Q18">
+        <v>1.8195517029999999</v>
+      </c>
+      <c r="R18" s="12">
+        <v>0.12987013</v>
+      </c>
+      <c r="S18">
+        <v>-2.7268544480000001</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>-1.58215003049999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>42199</v>
       </c>
@@ -2077,11 +2550,35 @@
       <c r="L19" s="4">
         <v>3.2085561497326109E-2</v>
       </c>
-      <c r="M19" s="3" t="s">
+      <c r="M19" s="14">
+        <v>-1.6759776536312887E-2</v>
+      </c>
+      <c r="N19" s="14">
+        <v>7.8212290502793325E-2</v>
+      </c>
+      <c r="O19" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P19" s="10">
+        <v>-6.7725145E-2</v>
+      </c>
+      <c r="Q19">
+        <v>2.33296097449999</v>
+      </c>
+      <c r="R19" s="12">
+        <v>-0.37561230199999901</v>
+      </c>
+      <c r="S19">
+        <v>-2.9856916333333299E-2</v>
+      </c>
+      <c r="T19">
+        <v>0.70422535200000003</v>
+      </c>
+      <c r="U19">
+        <v>-0.41240358433333302</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>42291</v>
       </c>
@@ -2118,11 +2615,35 @@
       <c r="L20" s="4">
         <v>8.1218274111675148E-2</v>
       </c>
-      <c r="M20" s="3" t="s">
+      <c r="M20" s="14">
+        <v>0.10309278350515472</v>
+      </c>
+      <c r="N20" s="14">
+        <v>9.7938144329896781E-2</v>
+      </c>
+      <c r="O20" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P20" s="10">
+        <v>0.46361995587499999</v>
+      </c>
+      <c r="Q20">
+        <v>2.7229092709999998</v>
+      </c>
+      <c r="R20" s="12">
+        <v>-0.94478117949999996</v>
+      </c>
+      <c r="S20">
+        <v>2.9142754999999899E-2</v>
+      </c>
+      <c r="T20">
+        <v>0.70422535200000003</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>42383</v>
       </c>
@@ -2159,11 +2680,35 @@
       <c r="L21" s="4">
         <v>2.051282051282044E-2</v>
       </c>
-      <c r="M21" s="3" t="s">
+      <c r="M21" s="14">
+        <v>0.14999999999999991</v>
+      </c>
+      <c r="N21" s="14">
+        <v>0.10555555555555562</v>
+      </c>
+      <c r="O21" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P21" s="10">
+        <v>1.349340132</v>
+      </c>
+      <c r="Q21">
+        <v>-2.4781341110000001</v>
+      </c>
+      <c r="R21" s="12">
+        <v>0.42735042699999998</v>
+      </c>
+      <c r="S21">
+        <v>-0.3798185945</v>
+      </c>
+      <c r="T21">
+        <v>0.70422535200000003</v>
+      </c>
+      <c r="U21">
+        <v>0.94843294449999904</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>42480</v>
       </c>
@@ -2200,11 +2745,35 @@
       <c r="L22" s="4">
         <v>0.39694656488549618</v>
       </c>
-      <c r="M22" s="3" t="s">
+      <c r="M22" s="14">
+        <v>-9.5238095238095344E-2</v>
+      </c>
+      <c r="N22" s="14">
+        <v>-8.2706766917293284E-2</v>
+      </c>
+      <c r="O22" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P22" s="10">
+        <v>1.7062187473333299</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22" s="12">
+        <v>0.104920634333333</v>
+      </c>
+      <c r="S22">
+        <v>-0.19762845800000001</v>
+      </c>
+      <c r="T22">
+        <v>0.70422535200000003</v>
+      </c>
+      <c r="U22">
+        <v>4.5454545450000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>42571</v>
       </c>
@@ -2241,11 +2810,35 @@
       <c r="L23" s="4">
         <v>0.23946360153256707</v>
       </c>
-      <c r="M23" s="3" t="s">
+      <c r="M23" s="14">
+        <v>0.16780821917808231</v>
+      </c>
+      <c r="N23" s="14">
+        <v>0.10787671232876717</v>
+      </c>
+      <c r="O23" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P23" s="10">
+        <v>1.5937800018999999</v>
+      </c>
+      <c r="Q23">
+        <v>1.214574899</v>
+      </c>
+      <c r="R23" s="12">
+        <v>0.85955510449999994</v>
+      </c>
+      <c r="S23">
+        <v>0.70237050000000001</v>
+      </c>
+      <c r="T23">
+        <v>0.70422535200000003</v>
+      </c>
+      <c r="U23">
+        <v>6.3583815030000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>42657</v>
       </c>
@@ -2282,11 +2875,35 @@
       <c r="L24" s="4">
         <v>-3.7356321839080442E-2</v>
       </c>
-      <c r="M24" s="3" t="s">
+      <c r="M24" s="14">
+        <v>9.0490797546012303E-2</v>
+      </c>
+      <c r="N24" s="14">
+        <v>2.7607361963190247E-2</v>
+      </c>
+      <c r="O24" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P24" s="10">
+        <v>2.4022516503888802</v>
+      </c>
+      <c r="Q24">
+        <v>2.7869996696666601</v>
+      </c>
+      <c r="R24" s="12">
+        <v>0.661014972888888</v>
+      </c>
+      <c r="S24">
+        <v>-0.76611668899999996</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>0.162821897133333</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>42765</v>
       </c>
@@ -2323,11 +2940,35 @@
       <c r="L25" s="4">
         <v>0.27868852459016402</v>
       </c>
-      <c r="M25" s="3" t="s">
+      <c r="M25" s="14">
+        <v>0.10199004975124359</v>
+      </c>
+      <c r="N25" s="14">
+        <v>9.9502487562189004E-2</v>
+      </c>
+      <c r="O25" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P25" s="10">
+        <v>0.67023551317241303</v>
+      </c>
+      <c r="Q25">
+        <v>2.27048197757142</v>
+      </c>
+      <c r="R25" s="12">
+        <v>3.3057579559999901</v>
+      </c>
+      <c r="S25">
+        <v>1.1699931180000001</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <v>1.07852101562499</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>42116</v>
       </c>
@@ -2364,11 +3005,35 @@
       <c r="L26" s="4">
         <v>-7.7159399740044932E-2</v>
       </c>
-      <c r="M26" s="3" t="s">
+      <c r="M26" s="14">
+        <v>-2.3662176920276723E-2</v>
+      </c>
+      <c r="N26" s="14">
+        <v>-5.2299478218662765E-2</v>
+      </c>
+      <c r="O26" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P26" s="10">
+        <v>0.19757342169505401</v>
+      </c>
+      <c r="Q26">
+        <v>8.9795241499999998E-2</v>
+      </c>
+      <c r="R26" s="12">
+        <v>-2.3048635549346699</v>
+      </c>
+      <c r="S26">
+        <v>-3.8759957775928502</v>
+      </c>
+      <c r="T26">
+        <v>-4.5865548269999996</v>
+      </c>
+      <c r="U26">
+        <v>0.23854339455172399</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>42214</v>
       </c>
@@ -2405,11 +3070,35 @@
       <c r="L27" s="4">
         <v>-2.8868955562429077E-2</v>
       </c>
-      <c r="M27" s="3" t="s">
+      <c r="M27" s="14">
+        <v>1.2918811049259515E-2</v>
+      </c>
+      <c r="N27" s="14">
+        <v>-1.0713160382312736E-2</v>
+      </c>
+      <c r="O27" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P27" s="10">
+        <v>1.0624828124833701</v>
+      </c>
+      <c r="Q27">
+        <v>-0.116786617985772</v>
+      </c>
+      <c r="R27" s="12">
+        <v>-1.27910615098606</v>
+      </c>
+      <c r="S27">
+        <v>-3.3686784756547801</v>
+      </c>
+      <c r="T27">
+        <v>-3.507256731</v>
+      </c>
+      <c r="U27">
+        <v>4.6677504861111101E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>42312</v>
       </c>
@@ -2446,11 +3135,35 @@
       <c r="L28" s="4">
         <v>3.6848181643255762E-2</v>
       </c>
-      <c r="M28" s="3" t="s">
+      <c r="M28" s="14">
+        <v>2.2986392055903693E-3</v>
+      </c>
+      <c r="N28" s="14">
+        <v>-9.1026112541375825E-3</v>
+      </c>
+      <c r="O28" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P28" s="10">
+        <v>1.16622926184237</v>
+      </c>
+      <c r="Q28">
+        <v>0.86937630060876303</v>
+      </c>
+      <c r="R28" s="12">
+        <v>0.30011461050731297</v>
+      </c>
+      <c r="S28">
+        <v>-2.4811846407974798</v>
+      </c>
+      <c r="T28">
+        <v>-2.3758590750000002</v>
+      </c>
+      <c r="U28">
+        <v>0.75347526535051501</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>42396</v>
       </c>
@@ -2487,11 +3200,35 @@
       <c r="L29" s="4">
         <v>6.9348861831656894E-2</v>
       </c>
-      <c r="M29" s="3" t="s">
+      <c r="M29" s="14">
+        <v>3.2810924754834492E-2</v>
+      </c>
+      <c r="N29" s="14">
+        <v>-7.4328659151315146E-2</v>
+      </c>
+      <c r="O29" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P29" s="10">
+        <v>0.91302616953879301</v>
+      </c>
+      <c r="Q29">
+        <v>0.75834462097142796</v>
+      </c>
+      <c r="R29" s="12">
+        <v>-1.6089773062636601</v>
+      </c>
+      <c r="S29">
+        <v>-3.0063040591884902</v>
+      </c>
+      <c r="T29">
+        <v>-2.8608090339999999</v>
+      </c>
+      <c r="U29">
+        <v>0.759386393891892</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>42487</v>
       </c>
@@ -2528,11 +3265,35 @@
       <c r="L30" s="4">
         <v>9.7621452842317824E-2</v>
       </c>
-      <c r="M30" s="3" t="s">
+      <c r="M30" s="14">
+        <v>1.1393814786258893E-2</v>
+      </c>
+      <c r="N30" s="14">
+        <v>2.3901310717039159E-2</v>
+      </c>
+      <c r="O30" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P30" s="10">
+        <v>0.93712775720334196</v>
+      </c>
+      <c r="Q30">
+        <v>-1.3641471843252</v>
+      </c>
+      <c r="R30" s="12">
+        <v>-0.81674635021814701</v>
+      </c>
+      <c r="S30">
+        <v>-2.2635088921267599</v>
+      </c>
+      <c r="T30">
+        <v>-3.4928980319999998</v>
+      </c>
+      <c r="U30">
+        <v>0.70791959966949103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>42578</v>
       </c>
@@ -2569,11 +3330,35 @@
       <c r="L31" s="5">
         <v>1.2485811577752415E-2</v>
       </c>
-      <c r="M31" s="3" t="s">
+      <c r="M31" s="15">
+        <v>-1.9919999999999938E-2</v>
+      </c>
+      <c r="N31" s="15">
+        <v>-9.6000000000007191E-4</v>
+      </c>
+      <c r="O31" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P31" s="10">
+        <v>0.84431231389384598</v>
+      </c>
+      <c r="Q31">
+        <v>0.203932997695082</v>
+      </c>
+      <c r="R31" s="12">
+        <v>-2.4277405174090201</v>
+      </c>
+      <c r="S31">
+        <v>-3.5791921342575002</v>
+      </c>
+      <c r="T31">
+        <v>-4.4641958329999998</v>
+      </c>
+      <c r="U31">
+        <v>0.14543667218978101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>42676</v>
       </c>
@@ -2610,11 +3395,35 @@
       <c r="L32" s="4">
         <v>-8.5161594715734812E-2</v>
       </c>
-      <c r="M32" s="3" t="s">
+      <c r="M32" s="14">
+        <v>2.6499999999999968E-2</v>
+      </c>
+      <c r="N32" s="14">
+        <v>-3.0499999999999972E-2</v>
+      </c>
+      <c r="O32" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P32" s="10">
+        <v>5.1809093500000701E-2</v>
+      </c>
+      <c r="Q32">
+        <v>-2.4036377818136998</v>
+      </c>
+      <c r="R32" s="12">
+        <v>-4.3295334635701703</v>
+      </c>
+      <c r="S32">
+        <v>-5.1664449799004002</v>
+      </c>
+      <c r="T32">
+        <v>-2.8853583409999999</v>
+      </c>
+      <c r="U32">
+        <v>-0.67469833894838704</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>42767</v>
       </c>
@@ -2651,11 +3460,35 @@
       <c r="L33" s="4">
         <v>1.5762215717181061E-3</v>
       </c>
-      <c r="M33" s="3" t="s">
+      <c r="M33" s="14">
+        <v>2.5680220116172325E-2</v>
+      </c>
+      <c r="N33" s="14">
+        <v>1.9871598899419141E-2</v>
+      </c>
+      <c r="O33" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P33" s="10">
+        <v>0.51677891176445401</v>
+      </c>
+      <c r="Q33">
+        <v>3.4475788373134399E-2</v>
+      </c>
+      <c r="R33" s="12">
+        <v>-2.6944464288117</v>
+      </c>
+      <c r="S33">
+        <v>-3.56870911451372</v>
+      </c>
+      <c r="T33">
+        <v>-3.6490568400000001</v>
+      </c>
+      <c r="U33">
+        <v>-0.82862476068902402</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>42116</v>
       </c>
@@ -2692,11 +3525,35 @@
       <c r="L34" s="4">
         <v>-2.979890310786093E-2</v>
       </c>
-      <c r="M34" s="3" t="s">
+      <c r="M34" s="14">
+        <v>-4.905673733762772E-2</v>
+      </c>
+      <c r="N34" s="14">
+        <v>-6.0807701836972927E-2</v>
+      </c>
+      <c r="O34" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P34" s="10">
+        <v>7.7473716305668003E-2</v>
+      </c>
+      <c r="Q34">
+        <v>1.78136408616745</v>
+      </c>
+      <c r="R34" s="12">
+        <v>-1.9061217151685399E-2</v>
+      </c>
+      <c r="S34">
+        <v>-0.889461611611428</v>
+      </c>
+      <c r="T34">
+        <v>-1.8205404329999999</v>
+      </c>
+      <c r="U34">
+        <v>0.10363041413207499</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>42200</v>
       </c>
@@ -2733,11 +3590,35 @@
       <c r="L35" s="4">
         <v>9.0954557213072329E-2</v>
       </c>
-      <c r="M35" s="3" t="s">
+      <c r="M35" s="14">
+        <v>-4.257500780170298E-2</v>
+      </c>
+      <c r="N35" s="14">
+        <v>-5.9946799815731033E-2</v>
+      </c>
+      <c r="O35" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P35" s="10">
+        <v>0.80307547969024096</v>
+      </c>
+      <c r="Q35">
+        <v>0.13255720861025599</v>
+      </c>
+      <c r="R35" s="12">
+        <v>0.60770918639060201</v>
+      </c>
+      <c r="S35">
+        <v>-2.4687035536448199</v>
+      </c>
+      <c r="T35">
+        <v>-3.0552243529999998</v>
+      </c>
+      <c r="U35">
+        <v>0.49300597138461499</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>42298</v>
       </c>
@@ -2774,11 +3655,35 @@
       <c r="L36" s="4">
         <v>0.12191043127387657</v>
       </c>
-      <c r="M36" s="3" t="s">
+      <c r="M36" s="14">
+        <v>2.1253561253561148E-2</v>
+      </c>
+      <c r="N36" s="14">
+        <v>4.1666666666666741E-2</v>
+      </c>
+      <c r="O36" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P36" s="10">
+        <v>1.0298958883877001</v>
+      </c>
+      <c r="Q36">
+        <v>1.27527568089795</v>
+      </c>
+      <c r="R36" s="12">
+        <v>0.61461647012083298</v>
+      </c>
+      <c r="S36">
+        <v>-1.46377817013793</v>
+      </c>
+      <c r="T36">
+        <v>-1.095640578</v>
+      </c>
+      <c r="U36">
+        <v>0.92751770686111001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>42396</v>
       </c>
@@ -2815,11 +3720,35 @@
       <c r="L37" s="4">
         <v>-8.1117021276595702E-2</v>
       </c>
-      <c r="M37" s="3" t="s">
+      <c r="M37" s="14">
+        <v>-0.10712090498921067</v>
+      </c>
+      <c r="N37" s="14">
+        <v>-9.6318577126790039E-2</v>
+      </c>
+      <c r="O37" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P37" s="10">
+        <v>0.39861546082045102</v>
+      </c>
+      <c r="Q37">
+        <v>-0.89054436032608697</v>
+      </c>
+      <c r="R37" s="12">
+        <v>-2.3867566602405099</v>
+      </c>
+      <c r="S37">
+        <v>-3.0795471895277702</v>
+      </c>
+      <c r="T37">
+        <v>-2.8661321960000001</v>
+      </c>
+      <c r="U37">
+        <v>3.5516258687499899E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>42480</v>
       </c>
@@ -2856,11 +3785,35 @@
       <c r="L38" s="4">
         <v>-7.6020233422030237E-2</v>
       </c>
-      <c r="M38" s="3" t="s">
+      <c r="M38" s="14">
+        <v>-3.8607621353144994E-2</v>
+      </c>
+      <c r="N38" s="14">
+        <v>-2.4124546099586808E-2</v>
+      </c>
+      <c r="O38" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P38" s="10">
+        <v>0.24900502890878301</v>
+      </c>
+      <c r="Q38">
+        <v>-5.7495980790697801E-2</v>
+      </c>
+      <c r="R38" s="12">
+        <v>0.145300451599119</v>
+      </c>
+      <c r="S38">
+        <v>-1.5684887270189201</v>
+      </c>
+      <c r="T38">
+        <v>-1.6352209</v>
+      </c>
+      <c r="U38">
+        <v>-0.89043110967123296</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>42578</v>
       </c>
@@ -2897,11 +3850,35 @@
       <c r="L39" s="4">
         <v>5.2204689573809304E-2</v>
       </c>
-      <c r="M39" s="3" t="s">
+      <c r="M39" s="14">
+        <v>3.6681018223443385E-3</v>
+      </c>
+      <c r="N39" s="14">
+        <v>2.0889969952782916E-2</v>
+      </c>
+      <c r="O39" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P39" s="10">
+        <v>0.59555566684465999</v>
+      </c>
+      <c r="Q39">
+        <v>0.40593112967961098</v>
+      </c>
+      <c r="R39" s="12">
+        <v>-0.35064499295636398</v>
+      </c>
+      <c r="S39">
+        <v>-1.72496839886363</v>
+      </c>
+      <c r="T39">
+        <v>-1.8423593</v>
+      </c>
+      <c r="U39">
+        <v>0.55678920755670003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>42669</v>
       </c>
@@ -2938,11 +3915,35 @@
       <c r="L40" s="4">
         <v>-4.1227132708870351E-2</v>
       </c>
-      <c r="M40" s="3" t="s">
+      <c r="M40" s="14">
+        <v>-4.1791870450230695E-2</v>
+      </c>
+      <c r="N40" s="14">
+        <v>-4.1251241560531615E-2</v>
+      </c>
+      <c r="O40" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P40" s="10">
+        <v>0.68846515702242095</v>
+      </c>
+      <c r="Q40">
+        <v>-0.30822078224999999</v>
+      </c>
+      <c r="R40" s="12">
+        <v>-0.15219786079015499</v>
+      </c>
+      <c r="S40">
+        <v>-2.0009379092285702</v>
+      </c>
+      <c r="T40">
+        <v>-1.408910863</v>
+      </c>
+      <c r="U40">
+        <v>-0.18575457568131801</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>42760</v>
       </c>
@@ -2979,11 +3980,35 @@
       <c r="L41" s="4">
         <v>-2.7146548098299639E-2</v>
       </c>
-      <c r="M41" s="3" t="s">
+      <c r="M41" s="14">
+        <v>-3.0098018972197549E-2</v>
+      </c>
+      <c r="N41" s="14">
+        <v>-1.6700878162539068E-2</v>
+      </c>
+      <c r="O41" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P41" s="10">
+        <v>0.89523567790871394</v>
+      </c>
+      <c r="Q41">
+        <v>-9.2129024456521699E-2</v>
+      </c>
+      <c r="R41" s="12">
+        <v>-2.5527951502925101</v>
+      </c>
+      <c r="S41">
+        <v>-1.9530840958193001</v>
+      </c>
+      <c r="T41">
+        <v>-2.2937228580000002</v>
+      </c>
+      <c r="U41">
+        <v>-8.4653060826923102E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>42109</v>
       </c>
@@ -3020,11 +4045,35 @@
       <c r="L42" s="4">
         <v>4.7002888781896957E-2</v>
       </c>
-      <c r="M42" s="3" t="s">
+      <c r="M42" s="14">
+        <v>3.9388773895044471E-2</v>
+      </c>
+      <c r="N42" s="14">
+        <v>5.9113600389626209E-2</v>
+      </c>
+      <c r="O42" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P42" s="10">
+        <v>1.46759335827814E-2</v>
+      </c>
+      <c r="Q42">
+        <v>1.0711666620908999</v>
+      </c>
+      <c r="R42" s="12">
+        <v>-0.50359946203940797</v>
+      </c>
+      <c r="S42">
+        <v>-0.88899956545312497</v>
+      </c>
+      <c r="T42">
+        <v>-1.2263414939999999</v>
+      </c>
+      <c r="U42">
+        <v>0.36417531372602702</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>42200</v>
       </c>
@@ -3061,11 +4110,35 @@
       <c r="L43" s="4">
         <v>-8.3766308740330198E-2</v>
       </c>
-      <c r="M43" s="3" t="s">
+      <c r="M43" s="14">
+        <v>-2.4529343226835087E-2</v>
+      </c>
+      <c r="N43" s="14">
+        <v>-2.6736984117250118E-2</v>
+      </c>
+      <c r="O43" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P43" s="10">
+        <v>-0.49030003080335599</v>
+      </c>
+      <c r="Q43">
+        <v>-0.90496337485401401</v>
+      </c>
+      <c r="R43" s="12">
+        <v>1.93298403071014</v>
+      </c>
+      <c r="S43">
+        <v>1.0317359495543399</v>
+      </c>
+      <c r="T43">
+        <v>1.030929244</v>
+      </c>
+      <c r="U43">
+        <v>-0.35733813542857101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>42291</v>
       </c>
@@ -3102,11 +4175,35 @@
       <c r="L44" s="4">
         <v>-5.9308403699235956E-2</v>
       </c>
-      <c r="M44" s="3" t="s">
+      <c r="M44" s="14">
+        <v>2.1473265073947756E-2</v>
+      </c>
+      <c r="N44" s="14">
+        <v>-1.9197952218428238E-3</v>
+      </c>
+      <c r="O44" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P44" s="10">
+        <v>-0.213943351425882</v>
+      </c>
+      <c r="Q44">
+        <v>-1.2292395640409799</v>
+      </c>
+      <c r="R44" s="12">
+        <v>1.77622825573003</v>
+      </c>
+      <c r="S44">
+        <v>0.72934145969047603</v>
+      </c>
+      <c r="T44">
+        <v>-1.876295056</v>
+      </c>
+      <c r="U44">
+        <v>0.31004300402222201</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>42382</v>
       </c>
@@ -3143,11 +4240,35 @@
       <c r="L45" s="4">
         <v>-4.0355944110530118E-2</v>
       </c>
-      <c r="M45" s="3" t="s">
+      <c r="M45" s="14">
+        <v>5.9904808796980014E-3</v>
+      </c>
+      <c r="N45" s="14">
+        <v>8.8626292466764678E-3</v>
+      </c>
+      <c r="O45" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P45" s="10">
+        <v>1.0527728745287299</v>
+      </c>
+      <c r="Q45">
+        <v>-0.29482407927777698</v>
+      </c>
+      <c r="R45" s="12">
+        <v>2.5149709972601602</v>
+      </c>
+      <c r="S45">
+        <v>-1.3453469701818099</v>
+      </c>
+      <c r="T45">
+        <v>-2.3597084320000001</v>
+      </c>
+      <c r="U45">
+        <v>0.71130678685000004</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>42473</v>
       </c>
@@ -3184,11 +4305,35 @@
       <c r="L46" s="4">
         <v>-4.7597193994623921E-2</v>
       </c>
-      <c r="M46" s="3" t="s">
+      <c r="M46" s="14">
+        <v>3.3402777777777892E-2</v>
+      </c>
+      <c r="N46" s="14">
+        <v>8.8194444444444908E-3</v>
+      </c>
+      <c r="O46" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P46" s="10">
+        <v>6.7699371570212996E-2</v>
+      </c>
+      <c r="Q46">
+        <v>-0.120215993633333</v>
+      </c>
+      <c r="R46" s="12">
+        <v>1.2999185532313999</v>
+      </c>
+      <c r="S46">
+        <v>-0.16367008411904699</v>
+      </c>
+      <c r="T46">
+        <v>-1.333218322</v>
+      </c>
+      <c r="U46">
+        <v>0.21350818588750001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>42564</v>
       </c>
@@ -3225,11 +4370,35 @@
       <c r="L47" s="4">
         <v>9.9462029275614317E-3</v>
       </c>
-      <c r="M47" s="3" t="s">
+      <c r="M47" s="14">
+        <v>1.9237999749341927E-2</v>
+      </c>
+      <c r="N47" s="14">
+        <v>1.1718260433638106E-2</v>
+      </c>
+      <c r="O47" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P47" s="10">
+        <v>1.05568580244502</v>
+      </c>
+      <c r="Q47">
+        <v>1.1134438230999899</v>
+      </c>
+      <c r="R47" s="12">
+        <v>1.7982152200566</v>
+      </c>
+      <c r="S47">
+        <v>-0.50213812410526304</v>
+      </c>
+      <c r="T47">
+        <v>-0.53961958700000001</v>
+      </c>
+      <c r="U47">
+        <v>1.0524094882333299</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>42655</v>
       </c>
@@ -3266,11 +4435,35 @@
       <c r="L48" s="4">
         <v>-6.9780965303354314E-3</v>
       </c>
-      <c r="M48" s="3" t="s">
+      <c r="M48" s="14">
+        <v>-9.9522292993636796E-4</v>
+      </c>
+      <c r="N48" s="14">
+        <v>1.9705414012738842E-2</v>
+      </c>
+      <c r="O48" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P48" s="10">
+        <v>1.5145824906923</v>
+      </c>
+      <c r="Q48">
+        <v>-0.2911722175</v>
+      </c>
+      <c r="R48" s="12">
+        <v>1.4412868003361301</v>
+      </c>
+      <c r="S48">
+        <v>-0.39104916369230702</v>
+      </c>
+      <c r="T48">
+        <v>0.240384615</v>
+      </c>
+      <c r="U48">
+        <v>0.99733154668420998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>42753</v>
       </c>
@@ -3307,11 +4500,35 @@
       <c r="L49" s="4">
         <v>4.6579941250524559E-2</v>
       </c>
-      <c r="M49" s="3" t="s">
+      <c r="M49" s="14">
+        <v>4.755203752565218E-2</v>
+      </c>
+      <c r="N49" s="14">
+        <v>2.3629434183523923E-2</v>
+      </c>
+      <c r="O49" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P49" s="10">
+        <v>0.73411523473099405</v>
+      </c>
+      <c r="Q49">
+        <v>1.9094907727999999</v>
+      </c>
+      <c r="R49" s="12">
+        <v>1.2470741773253</v>
+      </c>
+      <c r="S49">
+        <v>1.1712904994411699</v>
+      </c>
+      <c r="T49">
+        <v>2.203299989</v>
+      </c>
+      <c r="U49">
+        <v>0.81907345399999998</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>42102</v>
       </c>
@@ -3348,11 +4565,35 @@
       <c r="L50" s="4">
         <v>4.8586852969196626E-2</v>
       </c>
-      <c r="M50" s="3" t="s">
+      <c r="M50" s="14">
+        <v>-1.2183978068839418E-2</v>
+      </c>
+      <c r="N50" s="14">
+        <v>5.7873895826989763E-3</v>
+      </c>
+      <c r="O50" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P50" s="10">
+        <v>0.63781609562499997</v>
+      </c>
+      <c r="Q50">
+        <v>0.91388946538235305</v>
+      </c>
+      <c r="R50" s="12">
+        <v>1.31267112722413</v>
+      </c>
+      <c r="S50">
+        <v>3.5298201669411702</v>
+      </c>
+      <c r="T50">
+        <v>-1.706749418</v>
+      </c>
+      <c r="U50">
+        <v>0.116879043890411</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>42200</v>
       </c>
@@ -3389,11 +4630,35 @@
       <c r="L51" s="4">
         <v>-2.2903334456045754E-2</v>
       </c>
-      <c r="M51" s="3" t="s">
+      <c r="M51" s="14">
+        <v>-4.3478260869565077E-2</v>
+      </c>
+      <c r="N51" s="14">
+        <v>-2.9765886287625332E-2</v>
+      </c>
+      <c r="O51" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P51" s="10">
+        <v>0.24923907810138199</v>
+      </c>
+      <c r="Q51">
+        <v>2.18273873246428</v>
+      </c>
+      <c r="R51" s="12">
+        <v>1.0468154918630099</v>
+      </c>
+      <c r="S51">
+        <v>0.84634422428571399</v>
+      </c>
+      <c r="T51">
+        <v>-2.7869940309999999</v>
+      </c>
+      <c r="U51">
+        <v>9.9642176415093205E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>42284</v>
       </c>
@@ -3430,11 +4695,35 @@
       <c r="L52" s="4">
         <v>7.5842696629213391E-2</v>
       </c>
-      <c r="M52" s="3" t="s">
+      <c r="M52" s="14">
+        <v>1.9512195121951237E-2</v>
+      </c>
+      <c r="N52" s="14">
+        <v>5.0914634146341564E-2</v>
+      </c>
+      <c r="O52" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P52" s="10">
+        <v>0.85727296478333304</v>
+      </c>
+      <c r="Q52">
+        <v>3.2254323415999999</v>
+      </c>
+      <c r="R52" s="12">
+        <v>2.10639381625862</v>
+      </c>
+      <c r="S52">
+        <v>-0.99938021785714304</v>
+      </c>
+      <c r="T52">
+        <v>-5.4240631160000001</v>
+      </c>
+      <c r="U52">
+        <v>0.250146562898305</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>42382</v>
       </c>
@@ -3471,11 +4760,35 @@
       <c r="L53" s="4">
         <v>-5.2535125229077662E-2</v>
       </c>
-      <c r="M53" s="3" t="s">
+      <c r="M53" s="14">
+        <v>5.3763440860215006E-3</v>
+      </c>
+      <c r="N53" s="14">
+        <v>4.2338709677419262E-2</v>
+      </c>
+      <c r="O53" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P53" s="10">
+        <v>-3.4615894730061401E-2</v>
+      </c>
+      <c r="Q53">
+        <v>-1.2727757566315701</v>
+      </c>
+      <c r="R53" s="12">
+        <v>1.2690111207127599</v>
+      </c>
+      <c r="S53">
+        <v>-0.38448331259574398</v>
+      </c>
+      <c r="T53">
+        <v>-1.342281879</v>
+      </c>
+      <c r="U53">
+        <v>0.208658439770114</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>42473</v>
       </c>
@@ -3512,11 +4825,35 @@
       <c r="L54" s="4">
         <v>-3.9240506329114022E-2</v>
       </c>
-      <c r="M54" s="3" t="s">
+      <c r="M54" s="14">
+        <v>-1.8750000000000044E-2</v>
+      </c>
+      <c r="N54" s="14">
+        <v>-5.1250000000000018E-2</v>
+      </c>
+      <c r="O54" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P54" s="10">
+        <v>-0.252933227652892</v>
+      </c>
+      <c r="Q54">
+        <v>-0.67775134839999995</v>
+      </c>
+      <c r="R54" s="12">
+        <v>4.84059674796747E-3</v>
+      </c>
+      <c r="S54">
+        <v>-0.29561690331578899</v>
+      </c>
+      <c r="T54">
+        <v>-3.0242068130000002</v>
+      </c>
+      <c r="U54">
+        <v>1.05316817529411</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>42571</v>
       </c>
@@ -3553,11 +4890,35 @@
       <c r="L55" s="4">
         <v>-4.034743625665449E-2</v>
       </c>
-      <c r="M55" s="3" t="s">
+      <c r="M55" s="14">
+        <v>1.6340822877151995E-2</v>
+      </c>
+      <c r="N55" s="14">
+        <v>-5.836008170412299E-4</v>
+      </c>
+      <c r="O55" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P55" s="10">
+        <v>0.40690827706569299</v>
+      </c>
+      <c r="Q55">
+        <v>1.4695458900454501</v>
+      </c>
+      <c r="R55" s="12">
+        <v>0.97824792696428498</v>
+      </c>
+      <c r="S55">
+        <v>-0.555934405441176</v>
+      </c>
+      <c r="T55">
+        <v>-0.40550380200000002</v>
+      </c>
+      <c r="U55">
+        <v>-0.56476466363636302</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>42655</v>
       </c>
@@ -3594,11 +4955,35 @@
       <c r="L56" s="4">
         <v>-8.5562913907284655E-2</v>
       </c>
-      <c r="M56" s="3" t="s">
+      <c r="M56" s="14">
+        <v>-1.1546043368065195E-2</v>
+      </c>
+      <c r="N56" s="14">
+        <v>-2.787947057166984E-2</v>
+      </c>
+      <c r="O56" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P56" s="10">
+        <v>1.03342580048039</v>
+      </c>
+      <c r="Q56">
+        <v>-1.4596458111111E-2</v>
+      </c>
+      <c r="R56" s="12">
+        <v>0.62885264253448203</v>
+      </c>
+      <c r="S56">
+        <v>0.31002769623076898</v>
+      </c>
+      <c r="T56">
+        <v>-1.413441465</v>
+      </c>
+      <c r="U56">
+        <v>7.6572079012820496E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>42760</v>
       </c>
@@ -3635,11 +5020,35 @@
       <c r="L57" s="4">
         <v>-5.591054313099042E-2</v>
       </c>
-      <c r="M57" s="3" t="s">
+      <c r="M57" s="14">
+        <v>-3.4228541337546048E-2</v>
+      </c>
+      <c r="N57" s="14">
+        <v>-6.6350710900473842E-2</v>
+      </c>
+      <c r="O57" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P57" s="10">
+        <v>0.77013452453591102</v>
+      </c>
+      <c r="Q57">
+        <v>0.708474778653846</v>
+      </c>
+      <c r="R57" s="12">
+        <v>0.88069586800961497</v>
+      </c>
+      <c r="S57">
+        <v>-0.42594380705263102</v>
+      </c>
+      <c r="T57">
+        <v>-1.0084462030000001</v>
+      </c>
+      <c r="U57">
+        <v>0.99555330947272602</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>42095</v>
       </c>
@@ -3676,11 +5085,35 @@
       <c r="L58" s="4">
         <v>3.2436417250276461E-2</v>
       </c>
-      <c r="M58" s="3" t="s">
+      <c r="M58" s="14">
+        <v>4.1167664670658688E-2</v>
+      </c>
+      <c r="N58" s="14">
+        <v>4.8278443113772607E-2</v>
+      </c>
+      <c r="O58" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P58" s="10">
+        <v>0.170019370274193</v>
+      </c>
+      <c r="Q58">
+        <v>0.41850239430000002</v>
+      </c>
+      <c r="R58" s="12">
+        <v>0.4226340173</v>
+      </c>
+      <c r="S58">
+        <v>0.56980056999999995</v>
+      </c>
+      <c r="T58">
+        <v>3.0303030299999998</v>
+      </c>
+      <c r="U58">
+        <v>0.65718334074999996</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>42174</v>
       </c>
@@ -3717,11 +5150,35 @@
       <c r="L59" s="6">
         <v>-0.26852622814321392</v>
       </c>
-      <c r="M59" s="3" t="s">
+      <c r="M59" s="15">
+        <v>-3.0010172939979651E-2</v>
+      </c>
+      <c r="N59" s="15">
+        <v>-0.10630722278738558</v>
+      </c>
+      <c r="O59" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P59" s="10">
+        <v>0.56557370114634098</v>
+      </c>
+      <c r="Q59">
+        <v>0.4682017732</v>
+      </c>
+      <c r="R59" s="12">
+        <v>0.29666358833333301</v>
+      </c>
+      <c r="S59">
+        <v>4.44297502E-2</v>
+      </c>
+      <c r="T59">
+        <v>0</v>
+      </c>
+      <c r="U59">
+        <v>-1.1009318206666601</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>42273</v>
       </c>
@@ -3758,11 +5215,35 @@
       <c r="L60" s="6">
         <v>0.26337169939065674</v>
       </c>
-      <c r="M60" s="3" t="s">
+      <c r="M60" s="15">
+        <v>0.17661847894406035</v>
+      </c>
+      <c r="N60" s="15">
+        <v>0.17284726587052179</v>
+      </c>
+      <c r="O60" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P60" s="10">
+        <v>-0.25865091407142798</v>
+      </c>
+      <c r="Q60">
+        <v>1.3956550696666601</v>
+      </c>
+      <c r="R60" s="12">
+        <v>0.98278441699999897</v>
+      </c>
+      <c r="S60">
+        <v>-1.388888889</v>
+      </c>
+      <c r="T60">
+        <v>0</v>
+      </c>
+      <c r="U60">
+        <v>0.44462278975000002</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>42359</v>
       </c>
@@ -3799,11 +5280,35 @@
       <c r="L61" s="6">
         <v>-6.5023956194387389E-2</v>
       </c>
-      <c r="M61" s="3" t="s">
+      <c r="M61" s="15">
+        <v>-9.7902097902098362E-3</v>
+      </c>
+      <c r="N61" s="15">
+        <v>-4.4755244755244838E-2</v>
+      </c>
+      <c r="O61" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="62" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P61" s="10">
+        <v>0.24849302905691001</v>
+      </c>
+      <c r="Q61">
+        <v>2.3794564135999998</v>
+      </c>
+      <c r="R61" s="12">
+        <v>0.36286866833333298</v>
+      </c>
+      <c r="S61">
+        <v>0.61677916850000003</v>
+      </c>
+      <c r="T61">
+        <v>0.93676815000000002</v>
+      </c>
+      <c r="U61">
+        <v>-0.3353140255</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>42458</v>
       </c>
@@ -3840,11 +5345,35 @@
       <c r="L62" s="6">
         <v>3.8167938931297662E-2</v>
       </c>
-      <c r="M62" s="3" t="s">
+      <c r="M62" s="15">
+        <v>0</v>
+      </c>
+      <c r="N62" s="15">
+        <v>3.9159503342884427E-2</v>
+      </c>
+      <c r="O62" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="63" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P62" s="10">
+        <v>-1.33475223501449</v>
+      </c>
+      <c r="Q62">
+        <v>-4.4130626499999999E-2</v>
+      </c>
+      <c r="R62" s="12">
+        <v>-1.2764651522499999</v>
+      </c>
+      <c r="S62">
+        <v>1.19912146</v>
+      </c>
+      <c r="T62">
+        <v>-5.4054054049999998</v>
+      </c>
+      <c r="U62">
+        <v>8.2611050499999894E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>42549</v>
       </c>
@@ -3881,11 +5410,35 @@
       <c r="L63" s="6">
         <v>-4.5784883720930147E-2</v>
       </c>
-      <c r="M63" s="3" t="s">
+      <c r="M63" s="15">
+        <v>9.5999999999998309E-3</v>
+      </c>
+      <c r="N63" s="15">
+        <v>5.04E-2</v>
+      </c>
+      <c r="O63" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P63" s="10">
+        <v>-0.97681215696511603</v>
+      </c>
+      <c r="Q63">
+        <v>-1.5947933441428499</v>
+      </c>
+      <c r="R63" s="12">
+        <v>-0.46021489979999902</v>
+      </c>
+      <c r="S63">
+        <v>1.4012567828571401</v>
+      </c>
+      <c r="T63">
+        <v>0.139275766</v>
+      </c>
+      <c r="U63">
+        <v>-1.40965951749999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
         <v>42641</v>
       </c>
@@ -3922,11 +5475,35 @@
       <c r="L64" s="6">
         <v>-2.1910112359550538E-2</v>
       </c>
-      <c r="M64" s="3" t="s">
+      <c r="M64" s="15">
+        <v>-4.7457627118644097E-2</v>
+      </c>
+      <c r="N64" s="15">
+        <v>-1.6384180790960379E-2</v>
+      </c>
+      <c r="O64" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="65" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P64" s="10">
+        <v>0.37973069388371999</v>
+      </c>
+      <c r="Q64">
+        <v>2.7034485180000001</v>
+      </c>
+      <c r="R64" s="12">
+        <v>0.92031307900000003</v>
+      </c>
+      <c r="S64">
+        <v>1.282302829</v>
+      </c>
+      <c r="T64">
+        <v>0.139275766</v>
+      </c>
+      <c r="U64">
+        <v>-5.3421102954545399E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>42725</v>
       </c>
@@ -3963,11 +5540,35 @@
       <c r="L65" s="6">
         <v>7.0942662779397425E-2</v>
       </c>
-      <c r="M65" s="3" t="s">
+      <c r="M65" s="15">
+        <v>-3.9672272531263597E-2</v>
+      </c>
+      <c r="N65" s="15">
+        <v>-4.9590340664079413E-2</v>
+      </c>
+      <c r="O65" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P65" s="10">
+        <v>1.1571177130697601</v>
+      </c>
+      <c r="Q65">
+        <v>1.6559329763333299</v>
+      </c>
+      <c r="R65" s="12">
+        <v>1.1481862730000001</v>
+      </c>
+      <c r="S65">
+        <v>0.214709335999999</v>
+      </c>
+      <c r="T65">
+        <v>-1.174496644</v>
+      </c>
+      <c r="U65">
+        <v>1.3699792078064501</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
         <v>42816</v>
       </c>
@@ -4004,11 +5605,35 @@
       <c r="L66" s="6">
         <v>8.122402720060462E-2</v>
       </c>
-      <c r="M66" s="3" t="s">
+      <c r="M66" s="15">
+        <v>1.8994020400984857E-2</v>
+      </c>
+      <c r="N66" s="15">
+        <v>6.6830812521985195E-3</v>
+      </c>
+      <c r="O66" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P66" s="10">
+        <v>1.5560969091935399</v>
+      </c>
+      <c r="Q66">
+        <v>1.84921717042857</v>
+      </c>
+      <c r="R66" s="12">
+        <v>1.0798892563448199</v>
+      </c>
+      <c r="S66">
+        <v>0.735188117461538</v>
+      </c>
+      <c r="T66">
+        <v>0</v>
+      </c>
+      <c r="U66">
+        <v>1.0639142479130399</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
         <v>42116</v>
       </c>
@@ -4045,11 +5670,35 @@
       <c r="L67" s="6">
         <v>7.7526534379326328E-2</v>
       </c>
-      <c r="M67" s="3" t="s">
+      <c r="M67" s="15">
+        <v>1.6085230833507547E-2</v>
+      </c>
+      <c r="N67" s="15">
+        <v>-2.4441194902861785E-2</v>
+      </c>
+      <c r="O67" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P67" s="10">
+        <v>0.579793186579311</v>
+      </c>
+      <c r="Q67">
+        <v>2.2795738746153802</v>
+      </c>
+      <c r="R67" s="12">
+        <v>1.03653319431111</v>
+      </c>
+      <c r="S67">
+        <v>-1.17504332751785</v>
+      </c>
+      <c r="T67">
+        <v>-1.5944819480000001</v>
+      </c>
+      <c r="U67">
+        <v>0.70786676995555498</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
         <v>42200</v>
       </c>
@@ -4086,11 +5735,35 @@
       <c r="L68" s="6">
         <v>5.4991539763113995E-3</v>
       </c>
-      <c r="M68" s="3" t="s">
+      <c r="M68" s="15">
+        <v>-4.3917435221781931E-3</v>
+      </c>
+      <c r="N68" s="15">
+        <v>4.3917435221783041E-2</v>
+      </c>
+      <c r="O68" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="69" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P68" s="10">
+        <v>-3.6542122297071197E-2</v>
+      </c>
+      <c r="Q68">
+        <v>-0.36357152208333299</v>
+      </c>
+      <c r="R68" s="12">
+        <v>1.5250088626246101</v>
+      </c>
+      <c r="S68">
+        <v>-0.98934887838709595</v>
+      </c>
+      <c r="T68">
+        <v>-3.780515834</v>
+      </c>
+      <c r="U68">
+        <v>0.447982979189542</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>42298</v>
       </c>
@@ -4127,11 +5800,35 @@
       <c r="L69" s="6">
         <v>0.13220903601915479</v>
       </c>
-      <c r="M69" s="3" t="s">
+      <c r="M69" s="15">
+        <v>9.2680158880271701E-3</v>
+      </c>
+      <c r="N69" s="15">
+        <v>2.8560620389635138E-2</v>
+      </c>
+      <c r="O69" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="70" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P69" s="10">
+        <v>1.1038291182029301</v>
+      </c>
+      <c r="Q69">
+        <v>0.57724294791666597</v>
+      </c>
+      <c r="R69" s="12">
+        <v>1.11872564887019</v>
+      </c>
+      <c r="S69">
+        <v>0.23383809389690699</v>
+      </c>
+      <c r="T69">
+        <v>-2.101988849</v>
+      </c>
+      <c r="U69">
+        <v>0.80816773621686699</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>42396</v>
       </c>
@@ -4168,11 +5865,35 @@
       <c r="L70" s="6">
         <v>-4.5524394928928236E-2</v>
       </c>
-      <c r="M70" s="3" t="s">
+      <c r="M70" s="15">
+        <v>-5.6090034489018059E-2</v>
+      </c>
+      <c r="N70" s="15">
+        <v>-9.8021419495371354E-2</v>
+      </c>
+      <c r="O70" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P70" s="10">
+        <v>1.04381930486467</v>
+      </c>
+      <c r="Q70">
+        <v>-0.19916878067815999</v>
+      </c>
+      <c r="R70" s="12">
+        <v>1.5798780168164499</v>
+      </c>
+      <c r="S70">
+        <v>-0.52650869296190395</v>
+      </c>
+      <c r="T70">
+        <v>-1.1195201939999999</v>
+      </c>
+      <c r="U70">
+        <v>0.99382271365740704</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>42480</v>
       </c>
@@ -4209,11 +5930,35 @@
       <c r="L71" s="6">
         <v>-0.10469702402294734</v>
       </c>
-      <c r="M71" s="3" t="s">
+      <c r="M71" s="15">
+        <v>-3.6307454615681745E-2</v>
+      </c>
+      <c r="N71" s="15">
+        <v>-3.5534955581305594E-2</v>
+      </c>
+      <c r="O71" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="72" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P71" s="10">
+        <v>0.24499129063192801</v>
+      </c>
+      <c r="Q71">
+        <v>-0.83000133356097505</v>
+      </c>
+      <c r="R71" s="12">
+        <v>1.5908097956904701</v>
+      </c>
+      <c r="S71">
+        <v>-0.84440960238410501</v>
+      </c>
+      <c r="T71">
+        <v>-0.59250106899999999</v>
+      </c>
+      <c r="U71">
+        <v>-5.9707175238095399E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
         <v>42564</v>
       </c>
@@ -4250,11 +5995,35 @@
       <c r="L72" s="6">
         <v>6.5737427010736482E-2</v>
       </c>
-      <c r="M72" s="3" t="s">
+      <c r="M72" s="15">
+        <v>1.5203004829189792E-2</v>
+      </c>
+      <c r="N72" s="15">
+        <v>1.1983544983008354E-2</v>
+      </c>
+      <c r="O72" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="73" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P72" s="10">
+        <v>1.09620959407623</v>
+      </c>
+      <c r="Q72">
+        <v>1.4274314968999999</v>
+      </c>
+      <c r="R72" s="12">
+        <v>1.49803182088095</v>
+      </c>
+      <c r="S72">
+        <v>1.4013400770554E-2</v>
+      </c>
+      <c r="T72">
+        <v>1.0547688049999999</v>
+      </c>
+      <c r="U72">
+        <v>1.03163681874782</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
         <v>42662</v>
       </c>
@@ -4291,11 +6060,35 @@
       <c r="L73" s="6">
         <v>3.4235807860262035E-2</v>
       </c>
-      <c r="M73" s="3" t="s">
+      <c r="M73" s="15">
+        <v>7.3751257123702008E-3</v>
+      </c>
+      <c r="N73" s="15">
+        <v>-7.542742205832953E-3</v>
+      </c>
+      <c r="O73" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="74" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P73" s="10">
+        <v>1.21173380443599</v>
+      </c>
+      <c r="Q73">
+        <v>0.93361297865517201</v>
+      </c>
+      <c r="R73" s="12">
+        <v>1.41472235645114</v>
+      </c>
+      <c r="S73">
+        <v>-0.232052756734513</v>
+      </c>
+      <c r="T73">
+        <v>0.65656188299999996</v>
+      </c>
+      <c r="U73">
+        <v>0.83667480590604004</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>42760</v>
       </c>
@@ -4332,11 +6125,35 @@
       <c r="L74" s="6">
         <v>-3.2674653804262155E-3</v>
       </c>
-      <c r="M74" s="3" t="s">
+      <c r="M74" s="15">
+        <v>-3.9677713590757113E-2</v>
+      </c>
+      <c r="N74" s="15">
+        <v>-2.6147765278200064E-2</v>
+      </c>
+      <c r="O74" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="75" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P74" s="10">
+        <v>1.3447200355619799</v>
+      </c>
+      <c r="Q74">
+        <v>-0.13885877309375</v>
+      </c>
+      <c r="R74" s="12">
+        <v>0.53356370158713695</v>
+      </c>
+      <c r="S74">
+        <v>-0.75600192673412603</v>
+      </c>
+      <c r="T74">
+        <v>-2.294225365</v>
+      </c>
+      <c r="U74">
+        <v>0.80892977607317096</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
         <v>42109</v>
       </c>
@@ -4373,11 +6190,35 @@
       <c r="L75" s="6">
         <v>0.18389281507656063</v>
       </c>
-      <c r="M75" s="3" t="s">
+      <c r="M75" s="15">
+        <v>-7.7220077220078176E-3</v>
+      </c>
+      <c r="N75" s="15">
+        <v>1.4945821397434056E-3</v>
+      </c>
+      <c r="O75" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="76" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P75" s="10">
+        <v>0.29595765321184903</v>
+      </c>
+      <c r="Q75">
+        <v>-1.5745739049924199</v>
+      </c>
+      <c r="R75" s="12">
+        <v>2.2029454505382202</v>
+      </c>
+      <c r="S75" s="9">
+        <v>4.4970994684728698E-2</v>
+      </c>
+      <c r="T75">
+        <v>0.210641407</v>
+      </c>
+      <c r="U75">
+        <v>0.92159738031250005</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>42200</v>
       </c>
@@ -4414,11 +6255,35 @@
       <c r="L76" s="6">
         <v>9.1205543666564859E-2</v>
       </c>
-      <c r="M76" s="3" t="s">
+      <c r="M76" s="15">
+        <v>-3.7216129867887027E-2</v>
+      </c>
+      <c r="N76" s="15">
+        <v>-7.5382091356532288E-2</v>
+      </c>
+      <c r="O76" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="77" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P76" s="10">
+        <v>1.0151278504666601</v>
+      </c>
+      <c r="Q76">
+        <v>0.426344607352941</v>
+      </c>
+      <c r="R76" s="12">
+        <v>0.109800584952941</v>
+      </c>
+      <c r="S76" s="9">
+        <v>-0.91812453904651103</v>
+      </c>
+      <c r="T76">
+        <v>9.3484902999999994E-2</v>
+      </c>
+      <c r="U76">
+        <v>0.72393470754761902</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>42291</v>
       </c>
@@ -4455,11 +6320,35 @@
       <c r="L77" s="6">
         <v>-4.0188696362151943E-2</v>
       </c>
-      <c r="M77" s="3" t="s">
+      <c r="M77" s="15">
+        <v>-3.096250865565342E-2</v>
+      </c>
+      <c r="N77" s="15">
+        <v>4.6592145612820213E-2</v>
+      </c>
+      <c r="O77" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="78" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P77" s="10">
+        <v>-8.0043960249999893E-2</v>
+      </c>
+      <c r="Q77">
+        <v>-0.23276616110000001</v>
+      </c>
+      <c r="R77" s="12">
+        <v>-0.282578336672131</v>
+      </c>
+      <c r="S77" s="9">
+        <v>-1.3198511408172</v>
+      </c>
+      <c r="T77">
+        <v>-3.1199452870000002</v>
+      </c>
+      <c r="U77">
+        <v>5.7247521910112301E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
         <v>42382</v>
       </c>
@@ -4496,11 +6385,35 @@
       <c r="L78" s="6">
         <v>-0.1520066734637131</v>
       </c>
-      <c r="M78" s="3" t="s">
+      <c r="M78" s="15">
+        <v>-9.1980694263968821E-2</v>
+      </c>
+      <c r="N78" s="15">
+        <v>-0.15082606274364208</v>
+      </c>
+      <c r="O78" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="79" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P78" s="10">
+        <v>5.9072861238937202E-3</v>
+      </c>
+      <c r="Q78">
+        <v>-0.60801574866666597</v>
+      </c>
+      <c r="R78" s="12">
+        <v>-0.39769555312584998</v>
+      </c>
+      <c r="S78" s="9">
+        <v>-2.4136746196080399</v>
+      </c>
+      <c r="T78">
+        <v>-0.79161571500000005</v>
+      </c>
+      <c r="U78">
+        <v>8.6432613088235299E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>42473</v>
       </c>
@@ -4537,11 +6450,35 @@
       <c r="L79" s="6">
         <v>-0.14105166051660523</v>
       </c>
-      <c r="M79" s="3" t="s">
+      <c r="M79" s="15">
+        <v>-8.2679669281322532E-3</v>
+      </c>
+      <c r="N79" s="15">
+        <v>-1.3037947848208664E-2</v>
+      </c>
+      <c r="O79" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="80" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P79" s="10">
+        <v>3.0629214219178E-2</v>
+      </c>
+      <c r="Q79">
+        <v>-2.904257104</v>
+      </c>
+      <c r="R79" s="12">
+        <v>-0.309588909034334</v>
+      </c>
+      <c r="S79" s="9">
+        <v>-1.74291447527118</v>
+      </c>
+      <c r="T79">
+        <v>-2.1168012379999999</v>
+      </c>
+      <c r="U79">
+        <v>-0.45802052677777699</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>42564</v>
       </c>
@@ -4578,11 +6515,35 @@
       <c r="L80" s="6">
         <v>-4.4934723206153215E-2</v>
       </c>
-      <c r="M80" s="3" t="s">
+      <c r="M80" s="15">
+        <v>2.1202236719477963E-2</v>
+      </c>
+      <c r="N80" s="15">
+        <v>9.937092264678471E-2</v>
+      </c>
+      <c r="O80" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="81" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P80" s="10">
+        <v>-0.24322110133802799</v>
+      </c>
+      <c r="Q80">
+        <v>2.1882277447999998</v>
+      </c>
+      <c r="R80" s="12">
+        <v>0.421703518346774</v>
+      </c>
+      <c r="S80" s="9">
+        <v>-3.47906028562933</v>
+      </c>
+      <c r="T80">
+        <v>-1.56893471</v>
+      </c>
+      <c r="U80">
+        <v>-0.19633357195774601</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>42655</v>
       </c>
@@ -4619,11 +6580,35 @@
       <c r="L81" s="6">
         <v>0.25120240480961931</v>
       </c>
-      <c r="M81" s="3" t="s">
+      <c r="M81" s="15">
+        <v>7.1891573364761374E-2</v>
+      </c>
+      <c r="N81" s="15">
+        <v>5.118275949153972E-2</v>
+      </c>
+      <c r="O81" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="82" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P81" s="10">
+        <v>0.40348291835616401</v>
+      </c>
+      <c r="Q81">
+        <v>-1.30492386675</v>
+      </c>
+      <c r="R81" s="12">
+        <v>0.608163410474026</v>
+      </c>
+      <c r="S81" s="9">
+        <v>-1.4819208804905599</v>
+      </c>
+      <c r="T81">
+        <v>0.139879637</v>
+      </c>
+      <c r="U81">
+        <v>0.43605009203571399</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A82" s="2">
         <v>42753</v>
       </c>
@@ -4660,11 +6645,35 @@
       <c r="L82" s="6">
         <v>5.6431037070388879E-2</v>
       </c>
-      <c r="M82" s="3" t="s">
+      <c r="M82" s="15">
+        <v>8.019651759266111E-3</v>
+      </c>
+      <c r="N82" s="15">
+        <v>1.7123040242757102E-2</v>
+      </c>
+      <c r="O82" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="83" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P82" s="10">
+        <v>0.90596411689596501</v>
+      </c>
+      <c r="Q82">
+        <v>0.65782905155555504</v>
+      </c>
+      <c r="R82" s="12">
+        <v>0.71168547803089899</v>
+      </c>
+      <c r="S82" s="9">
+        <v>-1.19730083725563</v>
+      </c>
+      <c r="T82">
+        <v>-1.6740272469999999</v>
+      </c>
+      <c r="U82">
+        <v>1.1097643534397099</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A83" s="2">
         <v>42130</v>
       </c>
@@ -4701,11 +6710,35 @@
       <c r="L83" s="6">
         <v>-7.1142730102267571E-2</v>
       </c>
-      <c r="M83" s="3" t="s">
+      <c r="M83" s="15">
+        <v>2.2574447646493745E-2</v>
+      </c>
+      <c r="N83" s="15">
+        <v>3.3621517771373899E-3</v>
+      </c>
+      <c r="O83" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="84" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P83" s="10">
+        <v>0.44715458419999998</v>
+      </c>
+      <c r="Q83">
+        <v>0.394321119</v>
+      </c>
+      <c r="R83" s="12">
+        <v>0.57701077530769196</v>
+      </c>
+      <c r="S83" s="9">
+        <v>0.108657696428571</v>
+      </c>
+      <c r="T83">
+        <v>-3.0540767720000002</v>
+      </c>
+      <c r="U83">
+        <v>0.21125855718181799</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A84" s="2">
         <v>42221</v>
       </c>
@@ -4742,11 +6775,35 @@
       <c r="L84" s="6">
         <v>8.3618581907090483E-2</v>
       </c>
-      <c r="M84" s="3" t="s">
+      <c r="M84" s="15">
+        <v>2.3498694516971286E-2</v>
+      </c>
+      <c r="N84" s="15">
+        <v>-3.5683202785030455E-2</v>
+      </c>
+      <c r="O84" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="85" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P84" s="10">
+        <v>0.98486321743076899</v>
+      </c>
+      <c r="Q84">
+        <v>4.3309012693333298</v>
+      </c>
+      <c r="R84" s="12">
+        <v>1.4917280466923</v>
+      </c>
+      <c r="S84" s="9">
+        <v>-0.67846618693333305</v>
+      </c>
+      <c r="T84">
+        <v>0</v>
+      </c>
+      <c r="U84">
+        <v>0.58229982440000005</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
         <v>42307</v>
       </c>
@@ -4783,11 +6840,35 @@
       <c r="L85" s="6">
         <v>0.12306026705160589</v>
       </c>
-      <c r="M85" s="3" t="s">
+      <c r="M85" s="15">
+        <v>-3.6450079239302768E-2</v>
+      </c>
+      <c r="N85" s="15">
+        <v>-1.3629160063391432E-2</v>
+      </c>
+      <c r="O85" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="86" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P85" s="10">
+        <v>0.23954421090909001</v>
+      </c>
+      <c r="Q85">
+        <v>-8.5237714499999895E-2</v>
+      </c>
+      <c r="R85" s="12">
+        <v>1.6432443416</v>
+      </c>
+      <c r="S85" s="9">
+        <v>-1.0413831409999901</v>
+      </c>
+      <c r="T85">
+        <v>0</v>
+      </c>
+      <c r="U85">
+        <v>1.0713372731999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A86" s="2">
         <v>42412</v>
       </c>
@@ -4824,11 +6905,35 @@
       <c r="L86" s="6">
         <v>0.19088937093275482</v>
       </c>
-      <c r="M86" s="3" t="s">
+      <c r="M86" s="15">
+        <v>5.925432756324911E-2</v>
+      </c>
+      <c r="N86" s="15">
+        <v>9.6537949400798961E-2</v>
+      </c>
+      <c r="O86" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="87" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P86" s="10">
+        <v>0.7011901975</v>
+      </c>
+      <c r="Q86">
+        <v>0.27858032524999998</v>
+      </c>
+      <c r="R86" s="12">
+        <v>0.91032519275000001</v>
+      </c>
+      <c r="S86" s="9">
+        <v>-2.8907047579090901</v>
+      </c>
+      <c r="T86">
+        <v>-0.78003120100000001</v>
+      </c>
+      <c r="U86">
+        <v>1.68466350690476</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A87" s="2">
         <v>42496</v>
       </c>
@@ -4865,11 +6970,35 @@
       <c r="L87" s="6">
         <v>0.28338487489457398</v>
       </c>
-      <c r="M87" s="3" t="s">
+      <c r="M87" s="15">
+        <v>6.2713518789653477E-2</v>
+      </c>
+      <c r="N87" s="15">
+        <v>0.11395802830649093</v>
+      </c>
+      <c r="O87" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="88" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P87" s="10">
+        <v>0.33994753795238097</v>
+      </c>
+      <c r="Q87">
+        <v>-9.6142514833333206E-2</v>
+      </c>
+      <c r="R87" s="12">
+        <v>1.30619696270588</v>
+      </c>
+      <c r="S87" s="9">
+        <v>0.57556015685714201</v>
+      </c>
+      <c r="T87">
+        <v>-3.2786885250000002</v>
+      </c>
+      <c r="U87">
+        <v>1.16389307141025</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A88" s="2">
         <v>42587</v>
       </c>
@@ -4906,11 +7035,35 @@
       <c r="L88" s="6">
         <v>3.0653266331658324E-2</v>
       </c>
-      <c r="M88" s="3" t="s">
+      <c r="M88" s="15">
+        <v>-1.4911167512690282E-2</v>
+      </c>
+      <c r="N88" s="15">
+        <v>-2.3953045685279117E-2</v>
+      </c>
+      <c r="O88" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="89" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P88" s="10">
+        <v>1.25982939926315</v>
+      </c>
+      <c r="Q88">
+        <v>2.5980714385714201</v>
+      </c>
+      <c r="R88" s="12">
+        <v>1.4708423286666601</v>
+      </c>
+      <c r="S88" s="9">
+        <v>0.23612750900000001</v>
+      </c>
+      <c r="T88">
+        <v>1.7408123790000001</v>
+      </c>
+      <c r="U88">
+        <v>1.20751760637209</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A89" s="2">
         <v>42678</v>
       </c>
@@ -4947,11 +7100,35 @@
       <c r="L89" s="6">
         <v>0.38940534159657658</v>
       </c>
-      <c r="M89" s="3" t="s">
+      <c r="M89" s="15">
+        <v>5.024440150051146E-2</v>
+      </c>
+      <c r="N89" s="15">
+        <v>7.036489712401961E-2</v>
+      </c>
+      <c r="O89" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="90" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P89" s="10">
+        <v>0.91824426847499996</v>
+      </c>
+      <c r="Q89">
+        <v>1.218960614</v>
+      </c>
+      <c r="R89" s="12">
+        <v>1.0048169550999999</v>
+      </c>
+      <c r="S89" s="9">
+        <v>-0.66961171850000001</v>
+      </c>
+      <c r="T89">
+        <v>-0.354904412</v>
+      </c>
+      <c r="U89">
+        <v>2.1762630935999998</v>
+      </c>
+    </row>
+    <row r="90" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A90" s="2">
         <v>42769</v>
       </c>
@@ -4988,11 +7165,35 @@
       <c r="L90" s="6">
         <v>-0.12820072177350061</v>
       </c>
-      <c r="M90" s="3" t="s">
+      <c r="M90" s="15">
+        <v>-5.6064073226544608E-2</v>
+      </c>
+      <c r="N90" s="15">
+        <v>-0.1070234113712375</v>
+      </c>
+      <c r="O90" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="91" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P90" s="10">
+        <v>0.88465189463157901</v>
+      </c>
+      <c r="Q90">
+        <v>0.17325017349999999</v>
+      </c>
+      <c r="R90" s="12">
+        <v>1.32759501453333</v>
+      </c>
+      <c r="S90" s="9">
+        <v>1.35215837333333</v>
+      </c>
+      <c r="T90">
+        <v>1.648351648</v>
+      </c>
+      <c r="U90">
+        <v>-0.14461227341666599</v>
+      </c>
+    </row>
+    <row r="91" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A91" s="2">
         <v>42116</v>
       </c>
@@ -5029,11 +7230,35 @@
       <c r="L91" s="6">
         <v>-0.27777777777777768</v>
       </c>
-      <c r="M91" s="3" t="s">
+      <c r="M91" s="15">
+        <v>-0.10385616276318899</v>
+      </c>
+      <c r="N91" s="15">
+        <v>-0.11734090371421813</v>
+      </c>
+      <c r="O91" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="92" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P91" s="10">
+        <v>-0.15241820681972701</v>
+      </c>
+      <c r="Q91">
+        <v>-0.89691033321428504</v>
+      </c>
+      <c r="R91" s="12">
+        <v>-1.24895801883117E-2</v>
+      </c>
+      <c r="S91" s="9">
+        <v>-3.81262195006896</v>
+      </c>
+      <c r="T91">
+        <v>-5.6123968580000003</v>
+      </c>
+      <c r="U91">
+        <v>-1.43771071248571</v>
+      </c>
+    </row>
+    <row r="92" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A92" s="2">
         <v>42207</v>
       </c>
@@ -5070,11 +7295,35 @@
       <c r="L92" s="6">
         <v>-0.18938149972632723</v>
       </c>
-      <c r="M92" s="3" t="s">
+      <c r="M92" s="15">
+        <v>-6.0819462227912902E-2</v>
+      </c>
+      <c r="N92" s="15">
+        <v>-5.1856594110115117E-2</v>
+      </c>
+      <c r="O92" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="93" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P92" s="10">
+        <v>0.224592768081504</v>
+      </c>
+      <c r="Q92">
+        <v>-2.9027224176734601</v>
+      </c>
+      <c r="R92" s="12">
+        <v>-2.7752202457380499</v>
+      </c>
+      <c r="S92" s="9">
+        <v>-4.18945500727843</v>
+      </c>
+      <c r="T92">
+        <v>-2.3061094409999998</v>
+      </c>
+      <c r="U92">
+        <v>-0.305657584222222</v>
+      </c>
+    </row>
+    <row r="93" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A93" s="2">
         <v>42298</v>
       </c>
@@ -5111,11 +7360,35 @@
       <c r="L93" s="6">
         <v>-0.13688576898532223</v>
       </c>
-      <c r="M93" s="3" t="s">
+      <c r="M93" s="15">
+        <v>-5.6365403304178829E-2</v>
+      </c>
+      <c r="N93" s="15">
+        <v>-0.12374473598963398</v>
+      </c>
+      <c r="O93" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="94" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P93" s="10">
+        <v>7.2597818282809395E-2</v>
+      </c>
+      <c r="Q93">
+        <v>-1.18815333906818</v>
+      </c>
+      <c r="R93" s="12">
+        <v>-0.530750535414382</v>
+      </c>
+      <c r="S93" s="9">
+        <v>-3.3423148334305499</v>
+      </c>
+      <c r="T93">
+        <v>-2.3748689029999999</v>
+      </c>
+      <c r="U93">
+        <v>6.8111895000000006E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A94" s="2">
         <v>42410</v>
       </c>
@@ -5152,11 +7425,35 @@
       <c r="L94" s="6">
         <v>0.17423230974632831</v>
       </c>
-      <c r="M94" s="3" t="s">
+      <c r="M94" s="15">
+        <v>0.2879105520614953</v>
+      </c>
+      <c r="N94" s="15">
+        <v>0.22921034241788951</v>
+      </c>
+      <c r="O94" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="95" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P94" s="10">
+        <v>-0.94455879395579501</v>
+      </c>
+      <c r="Q94">
+        <v>0.74467172345833299</v>
+      </c>
+      <c r="R94" s="12">
+        <v>-0.79037361408137397</v>
+      </c>
+      <c r="S94" s="9">
+        <v>-2.7303788531238902</v>
+      </c>
+      <c r="T94">
+        <v>-2.1533287059999999</v>
+      </c>
+      <c r="U94">
+        <v>-0.70607758476666604</v>
+      </c>
+    </row>
+    <row r="95" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A95" s="2">
         <v>42480</v>
       </c>
@@ -5193,11 +7490,35 @@
       <c r="L95" s="6">
         <v>-0.17577464788732389</v>
       </c>
-      <c r="M95" s="3" t="s">
+      <c r="M95" s="15">
+        <v>-5.7200538358008091E-2</v>
+      </c>
+      <c r="N95" s="15">
+        <v>-1.5477792732166762E-2</v>
+      </c>
+      <c r="O95" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="96" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P95" s="10">
+        <v>-0.23605608441605799</v>
+      </c>
+      <c r="Q95">
+        <v>-0.12180157011538401</v>
+      </c>
+      <c r="R95" s="12">
+        <v>-1.01757233217424</v>
+      </c>
+      <c r="S95" s="9">
+        <v>-2.2924511941129899</v>
+      </c>
+      <c r="T95">
+        <v>-2.3184963999999999</v>
+      </c>
+      <c r="U95">
+        <v>-0.66192226828205103</v>
+      </c>
+    </row>
+    <row r="96" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A96" s="2">
         <v>42571</v>
       </c>
@@ -5234,11 +7555,35 @@
       <c r="L96" s="6">
         <v>1.2466124661246747E-2</v>
       </c>
-      <c r="M96" s="3" t="s">
+      <c r="M96" s="15">
+        <v>4.1217501585288696E-2</v>
+      </c>
+      <c r="N96" s="15">
+        <v>0.18452758402029179</v>
+      </c>
+      <c r="O96" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="97" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P96" s="10">
+        <v>-1.06564016465168</v>
+      </c>
+      <c r="Q96">
+        <v>-5.1511205681882304</v>
+      </c>
+      <c r="R96" s="12">
+        <v>-0.54308127575617204</v>
+      </c>
+      <c r="S96" s="9">
+        <v>-8.5240528235225792</v>
+      </c>
+      <c r="T96">
+        <v>-6.7605989329999998</v>
+      </c>
+      <c r="U96">
+        <v>-1.2145084312419301</v>
+      </c>
+    </row>
+    <row r="97" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A97" s="2">
         <v>42669</v>
       </c>
@@ -5275,11 +7620,35 @@
       <c r="L97" s="6">
         <v>0.10641989589358003</v>
       </c>
-      <c r="M97" s="3" t="s">
+      <c r="M97" s="15">
+        <v>1.2068965517241459E-2</v>
+      </c>
+      <c r="N97" s="15">
+        <v>9.9425287356321945E-2</v>
+      </c>
+      <c r="O97" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="98" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P97" s="10">
+        <v>-0.67584359159090801</v>
+      </c>
+      <c r="Q97">
+        <v>-1.9175480523361901</v>
+      </c>
+      <c r="R97" s="12">
+        <v>-1.27467381411303</v>
+      </c>
+      <c r="S97" s="9">
+        <v>-1.87279908825427</v>
+      </c>
+      <c r="T97">
+        <v>-1.348207194</v>
+      </c>
+      <c r="U97">
+        <v>-0.44088831684782498</v>
+      </c>
+    </row>
+    <row r="98" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A98" s="2">
         <v>42774</v>
       </c>
@@ -5316,11 +7685,35 @@
       <c r="L98" s="6">
         <v>-0.14369658119658113</v>
       </c>
-      <c r="M98" s="3" t="s">
+      <c r="M98" s="15">
+        <v>2.0109689213893889E-2</v>
+      </c>
+      <c r="N98" s="15">
+        <v>-2.3156611822059636E-2</v>
+      </c>
+      <c r="O98" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="99" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P98" s="10">
+        <v>-1.1753877835622599</v>
+      </c>
+      <c r="Q98">
+        <v>-1.17949306203773</v>
+      </c>
+      <c r="R98" s="12">
+        <v>-1.60944521919077</v>
+      </c>
+      <c r="S98" s="9">
+        <v>-2.2149997386442601</v>
+      </c>
+      <c r="T98">
+        <v>-3.4990859319999998</v>
+      </c>
+      <c r="U98">
+        <v>-1.3006242508923</v>
+      </c>
+    </row>
+    <row r="99" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A99" s="8">
         <v>42059</v>
       </c>
@@ -5357,11 +7750,35 @@
       <c r="L99" s="6">
         <v>-0.1512</v>
       </c>
-      <c r="M99" s="7" t="s">
+      <c r="M99" s="15">
+        <v>-2.8843380444188993E-3</v>
+      </c>
+      <c r="N99" s="15">
+        <v>-5.7686760888376098E-2</v>
+      </c>
+      <c r="O99" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P99" s="10">
+        <v>-0.25010539970742302</v>
+      </c>
+      <c r="Q99">
+        <v>1.06409506290909</v>
+      </c>
+      <c r="R99" s="12">
+        <v>-0.11793970435555499</v>
+      </c>
+      <c r="S99" s="9">
+        <v>-1.0023387654</v>
+      </c>
+      <c r="T99">
+        <v>-3.0898876400000002</v>
+      </c>
+      <c r="U99">
+        <v>0.2295910055</v>
+      </c>
+    </row>
+    <row r="100" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>42145</v>
       </c>
@@ -5398,11 +7815,35 @@
       <c r="L100" s="6">
         <v>-2.69E-2</v>
       </c>
-      <c r="M100" s="7" t="s">
+      <c r="M100" s="15">
+        <v>-3.9125431530494859E-2</v>
+      </c>
+      <c r="N100" s="15">
+        <v>-5.2934407364787051E-2</v>
+      </c>
+      <c r="O100" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P100" s="10">
+        <v>0.73184323828712805</v>
+      </c>
+      <c r="Q100">
+        <v>1.1879648618</v>
+      </c>
+      <c r="R100" s="12">
+        <v>-0.156534413101694</v>
+      </c>
+      <c r="S100" s="9">
+        <v>0.42049186620000001</v>
+      </c>
+      <c r="T100">
+        <v>-1.752023597</v>
+      </c>
+      <c r="U100">
+        <v>0.65796617019999903</v>
+      </c>
+    </row>
+    <row r="101" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>42236</v>
       </c>
@@ -5439,11 +7880,35 @@
       <c r="L101" s="6">
         <v>2.8500000000000001E-2</v>
       </c>
-      <c r="M101" s="7" t="s">
+      <c r="M101" s="15">
+        <v>1.1649071714597836E-2</v>
+      </c>
+      <c r="N101" s="15">
+        <v>2.4026210411357773E-2</v>
+      </c>
+      <c r="O101" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P101" s="10">
+        <v>-0.74487905975524404</v>
+      </c>
+      <c r="Q101">
+        <v>0.36573510214285698</v>
+      </c>
+      <c r="R101" s="12">
+        <v>-0.60167392442424195</v>
+      </c>
+      <c r="S101" s="9">
+        <v>-1.0511726342727199</v>
+      </c>
+      <c r="T101">
+        <v>-2.693602694</v>
+      </c>
+      <c r="U101">
+        <v>0.77782310799999999</v>
+      </c>
+    </row>
+    <row r="102" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>42332</v>
       </c>
@@ -5480,11 +7945,35 @@
       <c r="L102" s="6">
         <v>-0.17280000000000001</v>
       </c>
-      <c r="M102" s="7" t="s">
+      <c r="M102" s="15">
+        <v>-5.4588607594936778E-2</v>
+      </c>
+      <c r="N102" s="15">
+        <v>-4.1930379746835555E-2</v>
+      </c>
+      <c r="O102" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P102" s="10">
+        <v>0.11368135169124401</v>
+      </c>
+      <c r="Q102">
+        <v>-1.01024892996153</v>
+      </c>
+      <c r="R102" s="12">
+        <v>0.24596534759090899</v>
+      </c>
+      <c r="S102" s="9">
+        <v>-0.63518018699999901</v>
+      </c>
+      <c r="T102">
+        <v>-0.94194802399999999</v>
+      </c>
+      <c r="U102">
+        <v>-0.15878063974074</v>
+      </c>
+    </row>
+    <row r="103" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>42424</v>
       </c>
@@ -5521,11 +8010,35 @@
       <c r="L103" s="6">
         <v>4.99E-2</v>
       </c>
-      <c r="M103" s="7" t="s">
+      <c r="M103" s="15">
+        <v>5.415860735009681E-2</v>
+      </c>
+      <c r="N103" s="15">
+        <v>9.8646034816247452E-2</v>
+      </c>
+      <c r="O103" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P103" s="10">
+        <v>0.74743956725490102</v>
+      </c>
+      <c r="Q103">
+        <v>1.89563027284615</v>
+      </c>
+      <c r="R103" s="12">
+        <v>0.81926494703921504</v>
+      </c>
+      <c r="S103" s="9">
+        <v>1.549295775</v>
+      </c>
+      <c r="T103">
+        <v>-0.78048780500000003</v>
+      </c>
+      <c r="U103">
+        <v>-1.5400250366666599</v>
+      </c>
+    </row>
+    <row r="104" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>42515</v>
       </c>
@@ -5562,11 +8075,35 @@
       <c r="L104" s="6">
         <v>0.13439999999999999</v>
       </c>
-      <c r="M104" s="7" t="s">
+      <c r="M104" s="15">
+        <v>3.8343558282208701E-2</v>
+      </c>
+      <c r="N104" s="15">
+        <v>6.1349693251533832E-2</v>
+      </c>
+      <c r="O104" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P104" s="10">
+        <v>0.27750743619354801</v>
+      </c>
+      <c r="Q104">
+        <v>-1.0779750610000001</v>
+      </c>
+      <c r="R104" s="12">
+        <v>3.0071795928571399E-2</v>
+      </c>
+      <c r="S104" s="9">
+        <v>-0.97835408204545404</v>
+      </c>
+      <c r="T104">
+        <v>-0.83682985099999996</v>
+      </c>
+      <c r="U104">
+        <v>1.7809309303076899</v>
+      </c>
+    </row>
+    <row r="105" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>42606</v>
       </c>
@@ -5603,11 +8140,35 @@
       <c r="L105" s="6">
         <v>1.6E-2</v>
       </c>
-      <c r="M105" s="7" t="s">
+      <c r="M105" s="15">
+        <v>1E-4</v>
+      </c>
+      <c r="N105" s="15">
+        <v>1.8093249826026447E-2</v>
+      </c>
+      <c r="O105" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P105" s="10">
+        <v>1.0817459335283</v>
+      </c>
+      <c r="Q105">
+        <v>-0.70282204121052605</v>
+      </c>
+      <c r="R105" s="12">
+        <v>-0.27232927128947299</v>
+      </c>
+      <c r="S105" s="9">
+        <v>-2.2793224599999999</v>
+      </c>
+      <c r="T105">
+        <v>-3.8097304599999999</v>
+      </c>
+      <c r="U105">
+        <v>-4.0302467739130397E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>42696</v>
       </c>
@@ -5644,11 +8205,35 @@
       <c r="L106" s="6">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="M106" s="7" t="s">
+      <c r="M106" s="15">
+        <v>3.564223268325506E-2</v>
+      </c>
+      <c r="N106" s="15">
+        <v>8.6079354404841935E-2</v>
+      </c>
+      <c r="O106" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="P106" s="10">
+        <v>0.74624319918584003</v>
+      </c>
+      <c r="Q106">
+        <v>0.46834495152380901</v>
+      </c>
+      <c r="R106" s="12">
+        <v>0.71467335025000001</v>
+      </c>
+      <c r="S106" s="9">
+        <v>0.13899547570000001</v>
+      </c>
+      <c r="T106">
+        <v>-0.90462080099999997</v>
+      </c>
+      <c r="U106">
+        <v>-8.7027112500000003E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>42788</v>
       </c>
@@ -5677,25 +8262,44 @@
         <v>0.57527262656942268</v>
       </c>
       <c r="J107" s="6">
-        <v>-6.7699999999999996E-2</v>
+        <v>8.6418999999999996E-2</v>
       </c>
       <c r="K107" s="6">
-        <v>-3.4500000000000003E-2</v>
+        <v>8.7653999999999996E-2</v>
       </c>
       <c r="L107" s="6">
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="M107" s="7" t="s">
+        <v>6.9136000000000003E-2</v>
+      </c>
+      <c r="M107" s="15">
+        <v>1.1363636363637131E-3</v>
+      </c>
+      <c r="N107" s="15">
+        <v>-1.5909090909090984E-2</v>
+      </c>
+      <c r="O107" s="7" t="s">
         <v>6</v>
+      </c>
+      <c r="P107" s="10">
+        <v>0.46429957853124898</v>
+      </c>
+      <c r="Q107">
+        <v>2.3225835705</v>
+      </c>
+      <c r="R107" s="12">
+        <v>2.1753728750232502</v>
+      </c>
+      <c r="S107" s="9">
+        <v>1.3168188859999901</v>
+      </c>
+      <c r="T107">
+        <v>-1.1686143579999999</v>
+      </c>
+      <c r="U107">
+        <v>1.1050427147333299</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>